<commit_message>
T1.v3 - Teste final e commit final
</commit_message>
<xml_diff>
--- a/T1/resultados_Cholesky.xlsx
+++ b/T1/resultados_Cholesky.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,46 +384,70 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>tempo comp. Cholesky</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>norma2 sem Pivo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>determinante sem Pivo</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>tempo comp. sem Pivo</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>norma2 solucao Numpy</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>determinante solucao Numpy</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>tempo comp. sol. Numpy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3.14018491736755e-16</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>22724289.00000001</v>
+        <v>811801.0000000006</v>
       </c>
       <c r="D2" t="n">
-        <v>1.40135045340596</v>
+        <v>6.985664367675781e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>22724289</v>
+        <v>1.606934272667016</v>
       </c>
       <c r="F2" t="n">
-        <v>1.40135045340596</v>
+        <v>811800.999999998</v>
       </c>
       <c r="G2" t="n">
-        <v>22724289.00000003</v>
+        <v>2.932548522949219e-05</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.606934272667016</v>
+      </c>
+      <c r="I2" t="n">
+        <v>811800.9999999981</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5.769729614257812e-05</v>
       </c>
     </row>
     <row r="3">
@@ -431,22 +455,31 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.110223024625157e-16</v>
+        <v>8.000541662143798e-15</v>
       </c>
       <c r="C3" t="n">
-        <v>111279619396.0002</v>
+        <v>12449426929.00007</v>
       </c>
       <c r="D3" t="n">
-        <v>1.70781541122439</v>
+        <v>7.891654968261719e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>111279619396.0001</v>
+        <v>1.707792150386513</v>
       </c>
       <c r="F3" t="n">
-        <v>1.70781541122439</v>
+        <v>12449426929.00001</v>
       </c>
       <c r="G3" t="n">
-        <v>111279619396.0002</v>
+        <v>3.910064697265625e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.707792150386513</v>
+      </c>
+      <c r="I3" t="n">
+        <v>12449426928.99998</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3.910064697265625e-05</v>
       </c>
     </row>
     <row r="4">
@@ -454,22 +487,31 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.669031177528358e-15</v>
+        <v>1.499598997848221e-13</v>
       </c>
       <c r="C4" t="n">
-        <v>351856036246275.6</v>
+        <v>3642505846225.029</v>
       </c>
       <c r="D4" t="n">
-        <v>1.976099807537073</v>
+        <v>0.0001087188720703125</v>
       </c>
       <c r="E4" t="n">
-        <v>351856036246275.9</v>
+        <v>9.22858758939134</v>
       </c>
       <c r="F4" t="n">
-        <v>1.976099807537073</v>
+        <v>3642505846224.929</v>
       </c>
       <c r="G4" t="n">
-        <v>351856036246276.9</v>
+        <v>5.91278076171875e-05</v>
+      </c>
+      <c r="H4" t="n">
+        <v>9.228587589391163</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3642505846224.987</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3.4332275390625e-05</v>
       </c>
     </row>
     <row r="5">
@@ -477,22 +519,31 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>2.585604310932977e-14</v>
+        <v>1.855027013458529e-10</v>
       </c>
       <c r="C5" t="n">
-        <v>1.389462076969884e+16</v>
+        <v>37239773954134.3</v>
       </c>
       <c r="D5" t="n">
-        <v>2.27822389038878</v>
+        <v>0.0001480579376220703</v>
       </c>
       <c r="E5" t="n">
-        <v>1.389462076969894e+16</v>
+        <v>951.6137504317491</v>
       </c>
       <c r="F5" t="n">
-        <v>2.27822389038878</v>
+        <v>37239773953438.41</v>
       </c>
       <c r="G5" t="n">
-        <v>1.389462076969902e+16</v>
+        <v>8.368492126464844e-05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>951.6137504139588</v>
+      </c>
+      <c r="I5" t="n">
+        <v>37239773954134.29</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3.457069396972656e-05</v>
       </c>
     </row>
     <row r="6">
@@ -500,22 +551,31 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>1.216492397998459e-14</v>
+        <v>1.778922377480441e-14</v>
       </c>
       <c r="C6" t="n">
-        <v>1.436774426811852e+22</v>
+        <v>2.518612275825941e+21</v>
       </c>
       <c r="D6" t="n">
-        <v>2.438128959849348</v>
+        <v>0.0001931190490722656</v>
       </c>
       <c r="E6" t="n">
-        <v>1.436774426811854e+22</v>
+        <v>2.435596948390076</v>
       </c>
       <c r="F6" t="n">
-        <v>2.438128959849348</v>
+        <v>2.518612275825948e+21</v>
       </c>
       <c r="G6" t="n">
-        <v>1.43677442681186e+22</v>
+        <v>0.0001099109649658203</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.435596948390075</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.51861227582595e+21</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3.504753112792969e-05</v>
       </c>
     </row>
     <row r="7">
@@ -523,22 +583,31 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>5.4146340653429e-14</v>
+        <v>2.621137574964887e-14</v>
       </c>
       <c r="C7" t="n">
-        <v>2.521178667853367e+24</v>
+        <v>5.129658090748854e+25</v>
       </c>
       <c r="D7" t="n">
-        <v>2.753950239078262</v>
+        <v>0.000247955322265625</v>
       </c>
       <c r="E7" t="n">
-        <v>2.521178667853265e+24</v>
+        <v>2.594806261506959</v>
       </c>
       <c r="F7" t="n">
-        <v>2.753950239078274</v>
+        <v>5.129658090748897e+25</v>
       </c>
       <c r="G7" t="n">
-        <v>2.521178667853108e+24</v>
+        <v>0.0001435279846191406</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.59480626150696</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.129658090748888e+25</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3.647804260253906e-05</v>
       </c>
     </row>
     <row r="8">
@@ -546,22 +615,31 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1.138813398388645e-13</v>
+        <v>1.045733441113283e-14</v>
       </c>
       <c r="C8" t="n">
-        <v>6.886188953530566e+29</v>
+        <v>8.568046341833192e+27</v>
       </c>
       <c r="D8" t="n">
-        <v>2.816615949298362</v>
+        <v>0.0003144741058349609</v>
       </c>
       <c r="E8" t="n">
-        <v>6.886188953530475e+29</v>
+        <v>2.793486383530426</v>
       </c>
       <c r="F8" t="n">
-        <v>2.816615949298362</v>
+        <v>8.568046341833138e+27</v>
       </c>
       <c r="G8" t="n">
-        <v>6.886188953530514e+29</v>
+        <v>0.0001783370971679688</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.793486383530426</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8.568046341833212e+27</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3.957748413085938e-05</v>
       </c>
     </row>
     <row r="9">
@@ -569,22 +647,31 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>2.427481761514289e-14</v>
+        <v>3.523461519555973e-13</v>
       </c>
       <c r="C9" t="n">
-        <v>3.099275069420005e+31</v>
+        <v>2.679576537875895e+31</v>
       </c>
       <c r="D9" t="n">
-        <v>12.84585560614407</v>
+        <v>0.0003848075866699219</v>
       </c>
       <c r="E9" t="n">
-        <v>3.099275069422659e+31</v>
+        <v>17.98858265091783</v>
       </c>
       <c r="F9" t="n">
-        <v>12.84585560615852</v>
+        <v>2.679576537876005e+31</v>
       </c>
       <c r="G9" t="n">
-        <v>3.099275069418971e+31</v>
+        <v>0.0002229213714599609</v>
+      </c>
+      <c r="H9" t="n">
+        <v>17.98858265092075</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2.679576537875533e+31</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3.695487976074219e-05</v>
       </c>
     </row>
     <row r="10">
@@ -592,22 +679,31 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>7.327357659127654e-13</v>
+        <v>5.439579601525954e-13</v>
       </c>
       <c r="C10" t="n">
-        <v>3.143778866207146e+36</v>
+        <v>8.073525320320142e+35</v>
       </c>
       <c r="D10" t="n">
-        <v>4.732196026905648</v>
+        <v>0.0004799365997314453</v>
       </c>
       <c r="E10" t="n">
-        <v>3.143778866207615e+36</v>
+        <v>4.089790696438899</v>
       </c>
       <c r="F10" t="n">
-        <v>4.732196026905767</v>
+        <v>8.073525320321085e+35</v>
       </c>
       <c r="G10" t="n">
-        <v>3.143778866207464e+36</v>
+        <v>0.0002725124359130859</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4.089790696438723</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8.07352532032183e+35</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4.911422729492188e-05</v>
       </c>
     </row>
     <row r="11">
@@ -615,22 +711,31 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>4.669854473350391e-13</v>
+        <v>1.189849505328036e-12</v>
       </c>
       <c r="C11" t="n">
-        <v>6.121914049186459e+40</v>
+        <v>4.171031611536207e+39</v>
       </c>
       <c r="D11" t="n">
-        <v>3.36213850859877</v>
+        <v>0.0006587505340576172</v>
       </c>
       <c r="E11" t="n">
-        <v>6.121914049186606e+40</v>
+        <v>17.35729338441737</v>
       </c>
       <c r="F11" t="n">
-        <v>3.362138508598777</v>
+        <v>4.171031611535826e+39</v>
       </c>
       <c r="G11" t="n">
-        <v>6.121914049186304e+40</v>
+        <v>0.0003352165222167969</v>
+      </c>
+      <c r="H11" t="n">
+        <v>17.35729338443337</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4.171031611531885e+39</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9.918212890625e-05</v>
       </c>
     </row>
     <row r="12">
@@ -638,22 +743,31 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>8.728220377922274e-13</v>
+        <v>1.800188887067328e-11</v>
       </c>
       <c r="C12" t="n">
-        <v>7.200412428036623e+44</v>
+        <v>3.75768503856845e+42</v>
       </c>
       <c r="D12" t="n">
-        <v>5.477419708126742</v>
+        <v>0.001394748687744141</v>
       </c>
       <c r="E12" t="n">
-        <v>7.200412428036532e+44</v>
+        <v>24.23806724851069</v>
       </c>
       <c r="F12" t="n">
-        <v>5.477419708126398</v>
+        <v>3.757685038571573e+42</v>
       </c>
       <c r="G12" t="n">
-        <v>7.200412428037103e+44</v>
+        <v>0.0007874965667724609</v>
+      </c>
+      <c r="H12" t="n">
+        <v>24.23806724839061</v>
+      </c>
+      <c r="I12" t="n">
+        <v>3.757685038589905e+42</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.00011444091796875</v>
       </c>
     </row>
     <row r="13">
@@ -661,22 +775,31 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>6.625138435231928e-12</v>
+        <v>3.4837544270714e-13</v>
       </c>
       <c r="C13" t="n">
-        <v>1.465544845452036e+47</v>
+        <v>1.094466987402113e+47</v>
       </c>
       <c r="D13" t="n">
-        <v>6.27348893719399</v>
+        <v>0.0008699893951416016</v>
       </c>
       <c r="E13" t="n">
-        <v>1.465544845451943e+47</v>
+        <v>5.648290483218029</v>
       </c>
       <c r="F13" t="n">
-        <v>6.273488937193605</v>
+        <v>1.094466987402478e+47</v>
       </c>
       <c r="G13" t="n">
-        <v>1.465544845452083e+47</v>
+        <v>0.0004897117614746094</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5.6482904832174</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.094466987402749e+47</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0001423358917236328</v>
       </c>
     </row>
     <row r="14">
@@ -684,22 +807,31 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>6.990214558284331e-13</v>
+        <v>8.201347561477511e-14</v>
       </c>
       <c r="C14" t="n">
-        <v>1.841506763906326e+52</v>
+        <v>7.203368753278922e+54</v>
       </c>
       <c r="D14" t="n">
-        <v>7.983423605460515</v>
+        <v>0.0009775161743164062</v>
       </c>
       <c r="E14" t="n">
-        <v>1.841506763906659e+52</v>
+        <v>3.745807663783038</v>
       </c>
       <c r="F14" t="n">
-        <v>7.983423605461303</v>
+        <v>7.203368753278949e+54</v>
       </c>
       <c r="G14" t="n">
-        <v>1.841506763906416e+52</v>
+        <v>0.000522613525390625</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3.745807663783038</v>
+      </c>
+      <c r="I14" t="n">
+        <v>7.203368753279021e+54</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5.960464477539062e-05</v>
       </c>
     </row>
     <row r="15">
@@ -707,22 +839,31 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>6.259306264152599e-13</v>
+        <v>1.036637232883434e-09</v>
       </c>
       <c r="C15" t="n">
-        <v>6.606953407466264e+57</v>
+        <v>6.40347104687479e+53</v>
       </c>
       <c r="D15" t="n">
-        <v>4.018964754825189</v>
+        <v>0.001154661178588867</v>
       </c>
       <c r="E15" t="n">
-        <v>6.606953407465255e+57</v>
+        <v>4246.598294734663</v>
       </c>
       <c r="F15" t="n">
-        <v>4.018964754825203</v>
+        <v>6.403471047114816e+53</v>
       </c>
       <c r="G15" t="n">
-        <v>6.606953407465021e+57</v>
+        <v>0.0005393028259277344</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4246.598293908219</v>
+      </c>
+      <c r="I15" t="n">
+        <v>6.403471048360951e+53</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5.388259887695312e-05</v>
       </c>
     </row>
     <row r="16">
@@ -730,22 +871,31 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>1.534204013052576e-10</v>
+        <v>2.31370685832686e-12</v>
       </c>
       <c r="C16" t="n">
-        <v>8.936060045134579e+56</v>
+        <v>7.83098495134326e+60</v>
       </c>
       <c r="D16" t="n">
-        <v>1088.250010912468</v>
+        <v>0.001305341720581055</v>
       </c>
       <c r="E16" t="n">
-        <v>8.936060045770667e+56</v>
+        <v>63.08899475504415</v>
       </c>
       <c r="F16" t="n">
-        <v>1088.25001089442</v>
+        <v>7.830984951345365e+60</v>
       </c>
       <c r="G16" t="n">
-        <v>8.936060045919769e+56</v>
+        <v>0.0005953311920166016</v>
+      </c>
+      <c r="H16" t="n">
+        <v>63.08899475506855</v>
+      </c>
+      <c r="I16" t="n">
+        <v>7.830984951342824e+60</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.507469177246094e-05</v>
       </c>
     </row>
     <row r="17">
@@ -753,22 +903,31 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>9.058603503698634e-14</v>
+        <v>2.046263628128219e-12</v>
       </c>
       <c r="C17" t="n">
-        <v>3.144496509419687e+67</v>
+        <v>7.774210352096991e+62</v>
       </c>
       <c r="D17" t="n">
-        <v>4.115792984734029</v>
+        <v>0.001547098159790039</v>
       </c>
       <c r="E17" t="n">
-        <v>3.144496509419596e+67</v>
+        <v>8.278012055997321</v>
       </c>
       <c r="F17" t="n">
-        <v>4.115792984734029</v>
+        <v>7.774210352093635e+62</v>
       </c>
       <c r="G17" t="n">
-        <v>3.144496509419412e+67</v>
+        <v>0.000667572021484375</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8.278012055995735</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7.774210352097547e+62</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5.793571472167969e-05</v>
       </c>
     </row>
     <row r="18">
@@ -776,22 +935,31 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>4.288109060476344e-13</v>
+        <v>1.358096973651833e-10</v>
       </c>
       <c r="C18" t="n">
-        <v>6.299418933699943e+69</v>
+        <v>2.003483347477747e+67</v>
       </c>
       <c r="D18" t="n">
-        <v>4.252202662487867</v>
+        <v>0.004569768905639648</v>
       </c>
       <c r="E18" t="n">
-        <v>6.299418933700208e+69</v>
+        <v>6.5975934225286</v>
       </c>
       <c r="F18" t="n">
-        <v>4.252202662487866</v>
+        <v>2.003483347474869e+67</v>
       </c>
       <c r="G18" t="n">
-        <v>6.299418933700404e+69</v>
+        <v>0.002137660980224609</v>
+      </c>
+      <c r="H18" t="n">
+        <v>6.597593422530255</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2.003483347474182e+67</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.000125885009765625</v>
       </c>
     </row>
     <row r="19">
@@ -799,22 +967,31 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>1.164696379667119e-12</v>
+        <v>1.013967363057377e-13</v>
       </c>
       <c r="C19" t="n">
-        <v>4.244550612557215e+73</v>
+        <v>2.750689858298729e+74</v>
       </c>
       <c r="D19" t="n">
-        <v>4.450657678375359</v>
+        <v>0.005156755447387695</v>
       </c>
       <c r="E19" t="n">
-        <v>4.244550612556969e+73</v>
+        <v>4.361995134102214</v>
       </c>
       <c r="F19" t="n">
-        <v>4.450657678375357</v>
+        <v>2.750689858298881e+74</v>
       </c>
       <c r="G19" t="n">
-        <v>4.244550612557073e+73</v>
+        <v>0.002362489700317383</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4.361995134102216</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2.750689858298686e+74</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.0001251697540283203</v>
       </c>
     </row>
     <row r="20">
@@ -822,22 +999,31 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>2.359426417584126e-10</v>
+        <v>2.76733680660669e-10</v>
       </c>
       <c r="C20" t="n">
-        <v>1.561543016038234e+73</v>
+        <v>4.808210008653512e+74</v>
       </c>
       <c r="D20" t="n">
-        <v>669.3907573704631</v>
+        <v>0.005887746810913086</v>
       </c>
       <c r="E20" t="n">
-        <v>1.561543016024043e+73</v>
+        <v>91.5023845242263</v>
       </c>
       <c r="F20" t="n">
-        <v>669.3907573532093</v>
+        <v>4.808210008409245e+74</v>
       </c>
       <c r="G20" t="n">
-        <v>1.561543016062536e+73</v>
+        <v>0.002637386322021484</v>
+      </c>
+      <c r="H20" t="n">
+        <v>91.50238452309671</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4.808210008468947e+74</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0001366138458251953</v>
       </c>
     </row>
     <row r="21">
@@ -845,22 +1031,31 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>1.3849730844529e-12</v>
+        <v>6.054627505789501e-11</v>
       </c>
       <c r="C21" t="n">
-        <v>1.187583504380739e+81</v>
+        <v>1.297052066748948e+81</v>
       </c>
       <c r="D21" t="n">
-        <v>32.56273412325946</v>
+        <v>0.006605625152587891</v>
       </c>
       <c r="E21" t="n">
-        <v>1.187583504381194e+81</v>
+        <v>150.864593763022</v>
       </c>
       <c r="F21" t="n">
-        <v>32.56273412325477</v>
+        <v>1.29705206674521e+81</v>
       </c>
       <c r="G21" t="n">
-        <v>1.187583504381376e+81</v>
+        <v>0.002880573272705078</v>
+      </c>
+      <c r="H21" t="n">
+        <v>150.8645937634588</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1.297052066741504e+81</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0001306533813476562</v>
       </c>
     </row>
     <row r="22">
@@ -868,22 +1063,31 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>7.462238042058434e-11</v>
+        <v>1.880886477037752e-10</v>
       </c>
       <c r="C22" t="n">
-        <v>3.930602219984577e+85</v>
+        <v>3.744272979213227e+83</v>
       </c>
       <c r="D22" t="n">
-        <v>262.6694836412424</v>
+        <v>0.007464408874511719</v>
       </c>
       <c r="E22" t="n">
-        <v>3.930602219909798e+85</v>
+        <v>535.8838690149026</v>
       </c>
       <c r="F22" t="n">
-        <v>262.6694836417071</v>
+        <v>3.744272979043216e+83</v>
       </c>
       <c r="G22" t="n">
-        <v>3.930602219902667e+85</v>
+        <v>0.003165721893310547</v>
+      </c>
+      <c r="H22" t="n">
+        <v>535.883869031986</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3.744272978924728e+83</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0001320838928222656</v>
       </c>
     </row>
     <row r="23">
@@ -891,22 +1095,31 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>1.520718976484663e-11</v>
+        <v>1.825891293297175e-12</v>
       </c>
       <c r="C23" t="n">
-        <v>6.911873855844241e+89</v>
+        <v>1.45028900949697e+92</v>
       </c>
       <c r="D23" t="n">
-        <v>11.00942555966529</v>
+        <v>0.008332967758178711</v>
       </c>
       <c r="E23" t="n">
-        <v>6.911873855835549e+89</v>
+        <v>4.784842078780625</v>
       </c>
       <c r="F23" t="n">
-        <v>11.00942555965505</v>
+        <v>1.450289009497246e+92</v>
       </c>
       <c r="G23" t="n">
-        <v>6.911873855844681e+89</v>
+        <v>0.003452301025390625</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4.784842078780625</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1.450289009497316e+92</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.0001409053802490234</v>
       </c>
     </row>
     <row r="24">
@@ -914,22 +1127,31 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>5.101167816478232e-13</v>
+        <v>1.135907499779978e-10</v>
       </c>
       <c r="C24" t="n">
-        <v>5.445644166254698e+92</v>
+        <v>2.279646083948241e+93</v>
       </c>
       <c r="D24" t="n">
-        <v>44.40240139533652</v>
+        <v>0.00938725471496582</v>
       </c>
       <c r="E24" t="n">
-        <v>5.445644166255306e+92</v>
+        <v>155.3058689827857</v>
       </c>
       <c r="F24" t="n">
-        <v>44.40240139540724</v>
+        <v>2.27964608399781e+93</v>
       </c>
       <c r="G24" t="n">
-        <v>5.445644166245715e+92</v>
+        <v>0.003787040710449219</v>
+      </c>
+      <c r="H24" t="n">
+        <v>155.3058689851258</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2.279646083963636e+93</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.002804994583129883</v>
       </c>
     </row>
     <row r="25">
@@ -937,22 +1159,31 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>4.806232067865739e-12</v>
+        <v>2.834646218533476e-12</v>
       </c>
       <c r="C25" t="n">
-        <v>1.592846115335229e+99</v>
+        <v>1.328058644082522e+97</v>
       </c>
       <c r="D25" t="n">
-        <v>11.27780423515734</v>
+        <v>0.01133489608764648</v>
       </c>
       <c r="E25" t="n">
-        <v>1.592846115337566e+99</v>
+        <v>5.379997973112778</v>
       </c>
       <c r="F25" t="n">
-        <v>11.27780423516758</v>
+        <v>1.328058644084436e+97</v>
       </c>
       <c r="G25" t="n">
-        <v>1.59284611533566e+99</v>
+        <v>0.004102468490600586</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5.379997973112701</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.32805864408419e+97</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0001993179321289062</v>
       </c>
     </row>
     <row r="26">
@@ -960,22 +1191,31 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>8.607770182880783e-13</v>
+        <v>3.123899317305387e-12</v>
       </c>
       <c r="C26" t="n">
-        <v>6.390467141525434e+103</v>
+        <v>3.250023257561461e+102</v>
       </c>
       <c r="D26" t="n">
-        <v>6.650622999655762</v>
+        <v>0.01136159896850586</v>
       </c>
       <c r="E26" t="n">
-        <v>6.390467141525309e+103</v>
+        <v>5.250576972835259</v>
       </c>
       <c r="F26" t="n">
-        <v>6.650622999655686</v>
+        <v>3.250023257560635e+102</v>
       </c>
       <c r="G26" t="n">
-        <v>6.390467141525418e+103</v>
+        <v>0.004439115524291992</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5.250576972835288</v>
+      </c>
+      <c r="I26" t="n">
+        <v>3.250023257560464e+102</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.0001566410064697266</v>
       </c>
     </row>
     <row r="27">
@@ -983,22 +1223,31 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>7.009475657830047e-11</v>
+        <v>5.287360592543865e-12</v>
       </c>
       <c r="C27" t="n">
-        <v>4.76211957406742e+105</v>
+        <v>2.040042359044407e+107</v>
       </c>
       <c r="D27" t="n">
-        <v>280.8424173585562</v>
+        <v>0.0126805305480957</v>
       </c>
       <c r="E27" t="n">
-        <v>4.762119574018061e+105</v>
+        <v>8.796535256700455</v>
       </c>
       <c r="F27" t="n">
-        <v>280.8424173548809</v>
+        <v>2.040042359042814e+107</v>
       </c>
       <c r="G27" t="n">
-        <v>4.762119574079536e+105</v>
+        <v>0.004745721817016602</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8.796535256691179</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2.040042359045911e+107</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.0001780986785888672</v>
       </c>
     </row>
     <row r="28">
@@ -1006,22 +1255,31 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>2.159560188816143e-11</v>
+        <v>1.653541930717623e-11</v>
       </c>
       <c r="C28" t="n">
-        <v>9.612713683478099e+109</v>
+        <v>4.797403182337988e+111</v>
       </c>
       <c r="D28" t="n">
-        <v>122.9930560188701</v>
+        <v>0.01381874084472656</v>
       </c>
       <c r="E28" t="n">
-        <v>9.612713683344634e+109</v>
+        <v>12.46357414067869</v>
       </c>
       <c r="F28" t="n">
-        <v>122.9930560184373</v>
+        <v>4.797403182338475e+111</v>
       </c>
       <c r="G28" t="n">
-        <v>9.612713683376625e+109</v>
+        <v>0.00510716438293457</v>
+      </c>
+      <c r="H28" t="n">
+        <v>12.46357414068513</v>
+      </c>
+      <c r="I28" t="n">
+        <v>4.797403182335759e+111</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.0001828670501708984</v>
       </c>
     </row>
     <row r="29">
@@ -1029,22 +1287,31 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>9.948828267455313e-13</v>
+        <v>2.309711318461324e-12</v>
       </c>
       <c r="C29" t="n">
-        <v>2.835521610939429e+117</v>
+        <v>1.676771441443842e+118</v>
       </c>
       <c r="D29" t="n">
-        <v>7.6594314494679</v>
+        <v>0.01521706581115723</v>
       </c>
       <c r="E29" t="n">
-        <v>2.835521610939407e+117</v>
+        <v>5.769081349457414</v>
       </c>
       <c r="F29" t="n">
-        <v>7.659431449467601</v>
+        <v>1.676771441444299e+118</v>
       </c>
       <c r="G29" t="n">
-        <v>2.835521610939589e+117</v>
+        <v>0.00548100471496582</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5.769081349457416</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.676771441444281e+118</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.0001688003540039062</v>
       </c>
     </row>
     <row r="30">
@@ -1052,22 +1319,31 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>6.664593317218198e-11</v>
+        <v>1.351245301341664e-10</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0986926711623e+120</v>
+        <v>9.96983613809841e+118</v>
       </c>
       <c r="D30" t="n">
-        <v>112.4955855968486</v>
+        <v>0.01657605171203613</v>
       </c>
       <c r="E30" t="n">
-        <v>1.098692671157316e+120</v>
+        <v>235.2558803922626</v>
       </c>
       <c r="F30" t="n">
-        <v>112.4955855970528</v>
+        <v>9.969836139481465e+118</v>
       </c>
       <c r="G30" t="n">
-        <v>1.098692671155456e+120</v>
+        <v>0.005850553512573242</v>
+      </c>
+      <c r="H30" t="n">
+        <v>235.2558804016487</v>
+      </c>
+      <c r="I30" t="n">
+        <v>9.969836139085113e+118</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.0001819133758544922</v>
       </c>
     </row>
     <row r="31">
@@ -1075,22 +1351,31 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>2.741939462553047e-12</v>
+        <v>1.130925235834915e-10</v>
       </c>
       <c r="C31" t="n">
-        <v>2.435276706303103e+124</v>
+        <v>1.020613207155643e+121</v>
       </c>
       <c r="D31" t="n">
-        <v>15.89367315705537</v>
+        <v>0.01802945137023926</v>
       </c>
       <c r="E31" t="n">
-        <v>2.435276706304052e+124</v>
+        <v>1007.587675735851</v>
       </c>
       <c r="F31" t="n">
-        <v>15.89367315704969</v>
+        <v>1.020613207126407e+121</v>
       </c>
       <c r="G31" t="n">
-        <v>2.435276706304965e+124</v>
+        <v>0.006236553192138672</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1007.587675749527</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1.020613207112371e+121</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.0002124309539794922</v>
       </c>
     </row>
     <row r="32">
@@ -1098,22 +1383,31 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>1.765593264761521e-11</v>
+        <v>6.37898313335823e-12</v>
       </c>
       <c r="C32" t="n">
-        <v>2.483297574825814e+129</v>
+        <v>1.403452518247407e+129</v>
       </c>
       <c r="D32" t="n">
-        <v>6.044389417479255</v>
+        <v>0.01980781555175781</v>
       </c>
       <c r="E32" t="n">
-        <v>2.483297574826362e+129</v>
+        <v>11.56887242829396</v>
       </c>
       <c r="F32" t="n">
-        <v>6.044389417479228</v>
+        <v>1.40345251824679e+129</v>
       </c>
       <c r="G32" t="n">
-        <v>2.483297574824653e+129</v>
+        <v>0.006657600402832031</v>
+      </c>
+      <c r="H32" t="n">
+        <v>11.56887242829289</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1.403452518246926e+129</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.0002241134643554688</v>
       </c>
     </row>
     <row r="33">
@@ -1121,22 +1415,31 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>1.302220483183498e-10</v>
+        <v>5.681038297748872e-12</v>
       </c>
       <c r="C33" t="n">
-        <v>3.138919242460053e+134</v>
+        <v>1.187162776348539e+134</v>
       </c>
       <c r="D33" t="n">
-        <v>54.30517485241472</v>
+        <v>0.02129507064819336</v>
       </c>
       <c r="E33" t="n">
-        <v>3.138919242432164e+134</v>
+        <v>10.02571269005637</v>
       </c>
       <c r="F33" t="n">
-        <v>54.30517485219164</v>
+        <v>1.187162776348602e+134</v>
       </c>
       <c r="G33" t="n">
-        <v>3.138919242445204e+134</v>
+        <v>0.007094144821166992</v>
+      </c>
+      <c r="H33" t="n">
+        <v>10.02571269005756</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1.187162776348138e+134</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.0002341270446777344</v>
       </c>
     </row>
     <row r="34">
@@ -1144,22 +1447,31 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>1.461038972020089e-11</v>
+        <v>8.697545534603832e-10</v>
       </c>
       <c r="C34" t="n">
-        <v>1.236938438372286e+138</v>
+        <v>6.377910267313109e+134</v>
       </c>
       <c r="D34" t="n">
-        <v>16.99907244885591</v>
+        <v>0.02307844161987305</v>
       </c>
       <c r="E34" t="n">
-        <v>1.236938438375136e+138</v>
+        <v>5220.042517303313</v>
       </c>
       <c r="F34" t="n">
-        <v>16.99907244883267</v>
+        <v>6.377910271456635e+134</v>
       </c>
       <c r="G34" t="n">
-        <v>1.236938438377029e+138</v>
+        <v>0.007543563842773438</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5220.042515377251</v>
+      </c>
+      <c r="I34" t="n">
+        <v>6.377910273811176e+134</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.01932334899902344</v>
       </c>
     </row>
     <row r="35">
@@ -1167,22 +1479,31 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>6.351642006293825e-12</v>
+        <v>1.156525405383956e-11</v>
       </c>
       <c r="C35" t="n">
-        <v>7.25492413720753e+142</v>
+        <v>2.567505998246724e+144</v>
       </c>
       <c r="D35" t="n">
-        <v>9.918150722946256</v>
+        <v>0.02620077133178711</v>
       </c>
       <c r="E35" t="n">
-        <v>7.254924137209066e+142</v>
+        <v>9.900846754985738</v>
       </c>
       <c r="F35" t="n">
-        <v>9.918150722943929</v>
+        <v>2.567505998245769e+144</v>
       </c>
       <c r="G35" t="n">
-        <v>7.254924137211648e+142</v>
+        <v>0.007979393005371094</v>
+      </c>
+      <c r="H35" t="n">
+        <v>9.900846754985199</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2.567505998246276e+144</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.0002675056457519531</v>
       </c>
     </row>
     <row r="36">
@@ -1190,22 +1511,31 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>2.591761425691434e-12</v>
+        <v>2.952115596975779e-09</v>
       </c>
       <c r="C36" t="n">
-        <v>3.60249235232951e+147</v>
+        <v>6.480713373933916e+145</v>
       </c>
       <c r="D36" t="n">
-        <v>7.651880190185896</v>
+        <v>0.02681541442871094</v>
       </c>
       <c r="E36" t="n">
-        <v>3.602492352333091e+147</v>
+        <v>190.6716889818449</v>
       </c>
       <c r="F36" t="n">
-        <v>7.651880190184991</v>
+        <v>6.48071337342437e+145</v>
       </c>
       <c r="G36" t="n">
-        <v>3.602492352333807e+147</v>
+        <v>0.008424758911132812</v>
+      </c>
+      <c r="H36" t="n">
+        <v>190.6716889782593</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6.480713373551386e+145</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.0003042221069335938</v>
       </c>
     </row>
     <row r="37">
@@ -1213,22 +1543,31 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>3.294386515124031e-11</v>
+        <v>7.72383069134307e-12</v>
       </c>
       <c r="C37" t="n">
-        <v>6.270230998701178e+151</v>
+        <v>9.867337465713849e+151</v>
       </c>
       <c r="D37" t="n">
-        <v>11.64909355867772</v>
+        <v>0.02894234657287598</v>
       </c>
       <c r="E37" t="n">
-        <v>6.270230998725756e+151</v>
+        <v>15.61247357097661</v>
       </c>
       <c r="F37" t="n">
-        <v>11.64909355867947</v>
+        <v>9.867337465704661e+151</v>
       </c>
       <c r="G37" t="n">
-        <v>6.270230998725054e+151</v>
+        <v>0.008863449096679688</v>
+      </c>
+      <c r="H37" t="n">
+        <v>15.61247357097148</v>
+      </c>
+      <c r="I37" t="n">
+        <v>9.867337465711356e+151</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.0001935958862304688</v>
       </c>
     </row>
     <row r="38">
@@ -1236,22 +1575,31 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>1.278761805288354e-11</v>
+        <v>9.963262803867809e-12</v>
       </c>
       <c r="C38" t="n">
-        <v>2.954169801177039e+155</v>
+        <v>1.1468200448295e+156</v>
       </c>
       <c r="D38" t="n">
-        <v>27.95519022806743</v>
+        <v>0.03051495552062988</v>
       </c>
       <c r="E38" t="n">
-        <v>2.954169801128099e+155</v>
+        <v>22.69474611398114</v>
       </c>
       <c r="F38" t="n">
-        <v>27.95519022801933</v>
+        <v>1.146820044824589e+156</v>
       </c>
       <c r="G38" t="n">
-        <v>2.954169801132419e+155</v>
+        <v>0.009404897689819336</v>
+      </c>
+      <c r="H38" t="n">
+        <v>22.69474611391563</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1.146820044828239e+156</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.002206802368164062</v>
       </c>
     </row>
     <row r="39">
@@ -1259,22 +1607,31 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>8.272399956372847e-12</v>
+        <v>3.45774807405863e-11</v>
       </c>
       <c r="C39" t="n">
-        <v>1.618374351008324e+160</v>
+        <v>1.181908838049619e+160</v>
       </c>
       <c r="D39" t="n">
-        <v>71.42817027503663</v>
+        <v>0.03286218643188477</v>
       </c>
       <c r="E39" t="n">
-        <v>1.618374351002922e+160</v>
+        <v>30.59564414323118</v>
       </c>
       <c r="F39" t="n">
-        <v>71.42817027497055</v>
+        <v>1.181908838048603e+160</v>
       </c>
       <c r="G39" t="n">
-        <v>1.618374351004848e+160</v>
+        <v>0.009860038757324219</v>
+      </c>
+      <c r="H39" t="n">
+        <v>30.59564414324422</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1.181908838048345e+160</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.0002355575561523438</v>
       </c>
     </row>
     <row r="40">
@@ -1282,22 +1639,31 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>2.692026352227636e-10</v>
+        <v>3.97604775167782e-11</v>
       </c>
       <c r="C40" t="n">
-        <v>7.272551230269906e+163</v>
+        <v>1.646815408150893e+165</v>
       </c>
       <c r="D40" t="n">
-        <v>14.19303852384053</v>
+        <v>0.0357825756072998</v>
       </c>
       <c r="E40" t="n">
-        <v>7.272551230134311e+163</v>
+        <v>102.3151995581126</v>
       </c>
       <c r="F40" t="n">
-        <v>14.19303852371042</v>
+        <v>1.646815408163438e+165</v>
       </c>
       <c r="G40" t="n">
-        <v>7.272551230197366e+163</v>
+        <v>0.01047849655151367</v>
+      </c>
+      <c r="H40" t="n">
+        <v>102.315199557935</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1.646815408165977e+165</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.0002079010009765625</v>
       </c>
     </row>
     <row r="41">
@@ -1305,22 +1671,31 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>2.151302372171871e-11</v>
+        <v>4.862128308894213e-12</v>
       </c>
       <c r="C41" t="n">
-        <v>1.296694081660564e+170</v>
+        <v>7.839627956602134e+169</v>
       </c>
       <c r="D41" t="n">
-        <v>8.481518014707294</v>
+        <v>0.0363459587097168</v>
       </c>
       <c r="E41" t="n">
-        <v>1.296694081660495e+170</v>
+        <v>22.25536017600063</v>
       </c>
       <c r="F41" t="n">
-        <v>8.481518014706777</v>
+        <v>7.83962795664618e+169</v>
       </c>
       <c r="G41" t="n">
-        <v>1.296694081660599e+170</v>
+        <v>0.01146721839904785</v>
+      </c>
+      <c r="H41" t="n">
+        <v>22.2553601759416</v>
+      </c>
+      <c r="I41" t="n">
+        <v>7.839627956670463e+169</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.004471063613891602</v>
       </c>
     </row>
     <row r="42">
@@ -1328,22 +1703,31 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>2.015944798586861e-10</v>
+        <v>1.215055204458513e-12</v>
       </c>
       <c r="C42" t="n">
-        <v>7.300484635994363e+173</v>
+        <v>2.739716509410741e+177</v>
       </c>
       <c r="D42" t="n">
-        <v>141.7150474167377</v>
+        <v>0.04101109504699707</v>
       </c>
       <c r="E42" t="n">
-        <v>7.300484635958424e+173</v>
+        <v>6.731027340871297</v>
       </c>
       <c r="F42" t="n">
-        <v>141.7150474170567</v>
+        <v>2.73971650941064e+177</v>
       </c>
       <c r="G42" t="n">
-        <v>7.300484635943666e+173</v>
+        <v>0.01153063774108887</v>
+      </c>
+      <c r="H42" t="n">
+        <v>6.731027340871237</v>
+      </c>
+      <c r="I42" t="n">
+        <v>2.739716509410884e+177</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.0002675056457519531</v>
       </c>
     </row>
     <row r="43">
@@ -1351,22 +1735,31 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>2.902803313380385e-09</v>
+        <v>2.609511405388351e-12</v>
       </c>
       <c r="C43" t="n">
-        <v>1.712882890486379e+177</v>
+        <v>2.016951823384702e+180</v>
       </c>
       <c r="D43" t="n">
-        <v>367.7968170960179</v>
+        <v>0.04121494293212891</v>
       </c>
       <c r="E43" t="n">
-        <v>1.712882889688705e+177</v>
+        <v>8.230238073460065</v>
       </c>
       <c r="F43" t="n">
-        <v>367.7968170893785</v>
+        <v>2.01695182338463e+180</v>
       </c>
       <c r="G43" t="n">
-        <v>1.712882889717982e+177</v>
+        <v>0.01113677024841309</v>
+      </c>
+      <c r="H43" t="n">
+        <v>8.230238073460377</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2.016951823383919e+180</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.003707647323608398</v>
       </c>
     </row>
     <row r="44">
@@ -1374,22 +1767,31 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>2.883816722983357e-12</v>
+        <v>1.553831576328747e-12</v>
       </c>
       <c r="C44" t="n">
-        <v>5.464455262772729e+182</v>
+        <v>3.105107300543844e+183</v>
       </c>
       <c r="D44" t="n">
-        <v>16.12780602662725</v>
+        <v>0.04690766334533691</v>
       </c>
       <c r="E44" t="n">
-        <v>5.46445526276437e+182</v>
+        <v>8.82870939495468</v>
       </c>
       <c r="F44" t="n">
-        <v>16.1278060266417</v>
+        <v>3.105107300544484e+183</v>
       </c>
       <c r="G44" t="n">
-        <v>5.464455262758642e+182</v>
+        <v>0.01293778419494629</v>
+      </c>
+      <c r="H44" t="n">
+        <v>8.828709394954851</v>
+      </c>
+      <c r="I44" t="n">
+        <v>3.105107300543561e+183</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.002388477325439453</v>
       </c>
     </row>
     <row r="45">
@@ -1397,22 +1799,31 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>4.496694004520353e-11</v>
+        <v>1.765618278835887e-11</v>
       </c>
       <c r="C45" t="n">
-        <v>9.865399867319468e+187</v>
+        <v>3.502773810759635e+188</v>
       </c>
       <c r="D45" t="n">
-        <v>16.2515330277014</v>
+        <v>0.04789161682128906</v>
       </c>
       <c r="E45" t="n">
-        <v>9.86539986731379e+187</v>
+        <v>13.79620328815041</v>
       </c>
       <c r="F45" t="n">
-        <v>16.25153302770368</v>
+        <v>3.502773810752344e+188</v>
       </c>
       <c r="G45" t="n">
-        <v>9.865399867297868e+187</v>
+        <v>0.01355624198913574</v>
+      </c>
+      <c r="H45" t="n">
+        <v>13.79620328813679</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3.502773810757115e+188</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.01420021057128906</v>
       </c>
     </row>
     <row r="46">
@@ -1420,22 +1831,31 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>2.799060348641778e-10</v>
+        <v>1.060094484890893e-11</v>
       </c>
       <c r="C46" t="n">
-        <v>7.068467610156223e+188</v>
+        <v>2.098594214371075e+193</v>
       </c>
       <c r="D46" t="n">
-        <v>46.14543445643952</v>
+        <v>0.05300378799438477</v>
       </c>
       <c r="E46" t="n">
-        <v>7.068467610575474e+188</v>
+        <v>8.246810972491643</v>
       </c>
       <c r="F46" t="n">
-        <v>46.14543445967323</v>
+        <v>2.098594214373013e+193</v>
       </c>
       <c r="G46" t="n">
-        <v>7.068467610092028e+188</v>
+        <v>0.01386189460754395</v>
+      </c>
+      <c r="H46" t="n">
+        <v>8.246810972491607</v>
+      </c>
+      <c r="I46" t="n">
+        <v>2.098594214373903e+193</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.0006158351898193359</v>
       </c>
     </row>
     <row r="47">
@@ -1443,22 +1863,31 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>2.572684498677024e-11</v>
+        <v>2.833776104147416e-11</v>
       </c>
       <c r="C47" t="n">
-        <v>1.240411705942714e+196</v>
+        <v>1.856473146826689e+197</v>
       </c>
       <c r="D47" t="n">
-        <v>8.874939845216746</v>
+        <v>0.05462002754211426</v>
       </c>
       <c r="E47" t="n">
-        <v>1.24041170594337e+196</v>
+        <v>75.39562718105854</v>
       </c>
       <c r="F47" t="n">
-        <v>8.874939845204761</v>
+        <v>1.856473146830697e+197</v>
       </c>
       <c r="G47" t="n">
-        <v>1.240411705943243e+196</v>
+        <v>0.01446223258972168</v>
+      </c>
+      <c r="H47" t="n">
+        <v>75.39562718063618</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1.856473146845018e+197</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.002922534942626953</v>
       </c>
     </row>
     <row r="48">
@@ -1466,22 +1895,31 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>9.955419765456981e-09</v>
+        <v>1.137198848054318e-11</v>
       </c>
       <c r="C48" t="n">
-        <v>1.030479629625208e+201</v>
+        <v>1.922745016102448e+199</v>
       </c>
       <c r="D48" t="n">
-        <v>2078.736188494825</v>
+        <v>0.05800080299377441</v>
       </c>
       <c r="E48" t="n">
-        <v>1.030479629735918e+201</v>
+        <v>292.4459021324018</v>
       </c>
       <c r="F48" t="n">
-        <v>2078.736188552585</v>
+        <v>1.922745016103248e+199</v>
       </c>
       <c r="G48" t="n">
-        <v>1.030479629707544e+201</v>
+        <v>0.0148160457611084</v>
+      </c>
+      <c r="H48" t="n">
+        <v>292.445902129403</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1.922745016123422e+199</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.0007145404815673828</v>
       </c>
     </row>
     <row r="49">
@@ -1489,22 +1927,31 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>5.815144689271194e-12</v>
+        <v>1.96733272391441e-11</v>
       </c>
       <c r="C49" t="n">
-        <v>1.358998287413189e+207</v>
+        <v>1.039090346757568e+207</v>
       </c>
       <c r="D49" t="n">
-        <v>32.90796941544757</v>
+        <v>0.06125378608703613</v>
       </c>
       <c r="E49" t="n">
-        <v>1.358998287424141e+207</v>
+        <v>20.43626845483987</v>
       </c>
       <c r="F49" t="n">
-        <v>32.90796941545096</v>
+        <v>1.039090346756297e+207</v>
       </c>
       <c r="G49" t="n">
-        <v>1.358998287423207e+207</v>
+        <v>0.01511693000793457</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20.43626845485112</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1.039090346755682e+207</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.003651142120361328</v>
       </c>
     </row>
     <row r="50">
@@ -1512,22 +1959,31 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>1.049232315578647e-11</v>
+        <v>4.862936514571985e-12</v>
       </c>
       <c r="C50" t="n">
-        <v>2.385390707279811e+211</v>
+        <v>7.501344654747801e+212</v>
       </c>
       <c r="D50" t="n">
-        <v>7.223025597188681</v>
+        <v>0.06592416763305664</v>
       </c>
       <c r="E50" t="n">
-        <v>2.385390707282889e+211</v>
+        <v>9.031916940090925</v>
       </c>
       <c r="F50" t="n">
-        <v>7.22302559718883</v>
+        <v>7.501344654748516e+212</v>
       </c>
       <c r="G50" t="n">
-        <v>2.385390707279177e+211</v>
+        <v>0.01635169982910156</v>
+      </c>
+      <c r="H50" t="n">
+        <v>9.031916940090747</v>
+      </c>
+      <c r="I50" t="n">
+        <v>7.501344654748873e+212</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.00035858154296875</v>
       </c>
     </row>
     <row r="51">
@@ -1535,22 +1991,31 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>6.742597011060358e-12</v>
+        <v>1.8354862742594e-12</v>
       </c>
       <c r="C51" t="n">
-        <v>8.256118828212906e+216</v>
+        <v>3.56502276811121e+217</v>
       </c>
       <c r="D51" t="n">
-        <v>8.022843369469152</v>
+        <v>0.07045769691467285</v>
       </c>
       <c r="E51" t="n">
-        <v>8.25611882822042e+216</v>
+        <v>7.38188461168671</v>
       </c>
       <c r="F51" t="n">
-        <v>8.022843369469108</v>
+        <v>3.565022768111285e+217</v>
       </c>
       <c r="G51" t="n">
-        <v>8.25611882822113e+216</v>
+        <v>0.01696372032165527</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7.381884611686795</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3.565022768111797e+217</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.0003619194030761719</v>
       </c>
     </row>
     <row r="52">
@@ -1558,22 +2023,31 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>6.711177148463861e-10</v>
+        <v>4.747069680867027e-11</v>
       </c>
       <c r="C52" t="n">
-        <v>1.07161407508671e+217</v>
+        <v>7.898486277249778e+218</v>
       </c>
       <c r="D52" t="n">
-        <v>75.74421252313755</v>
+        <v>0.07393193244934082</v>
       </c>
       <c r="E52" t="n">
-        <v>1.071614075150547e+217</v>
+        <v>26.57285857193972</v>
       </c>
       <c r="F52" t="n">
-        <v>75.74421252351314</v>
+        <v>7.898486277299917e+218</v>
       </c>
       <c r="G52" t="n">
-        <v>1.071614075141834e+217</v>
+        <v>0.01766681671142578</v>
+      </c>
+      <c r="H52" t="n">
+        <v>26.57285857204568</v>
+      </c>
+      <c r="I52" t="n">
+        <v>7.898486277263691e+218</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.0004034042358398438</v>
       </c>
     </row>
     <row r="53">
@@ -1581,22 +2055,31 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>1.455224349440059e-11</v>
+        <v>8.366385716387523e-12</v>
       </c>
       <c r="C53" t="n">
-        <v>1.921903593217267e+223</v>
+        <v>2.153180639734884e+225</v>
       </c>
       <c r="D53" t="n">
-        <v>69.57131783320304</v>
+        <v>0.07829594612121582</v>
       </c>
       <c r="E53" t="n">
-        <v>1.9219035932209e+223</v>
+        <v>8.380340325102752</v>
       </c>
       <c r="F53" t="n">
-        <v>69.57131783327623</v>
+        <v>2.153180639737639e+225</v>
       </c>
       <c r="G53" t="n">
-        <v>1.921903593217921e+223</v>
+        <v>0.01834440231323242</v>
+      </c>
+      <c r="H53" t="n">
+        <v>8.380340325103706</v>
+      </c>
+      <c r="I53" t="n">
+        <v>2.153180639736777e+225</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.0003948211669921875</v>
       </c>
     </row>
     <row r="54">
@@ -1604,22 +2087,31 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>4.357150866651226e-11</v>
+        <v>6.52722784046799e-11</v>
       </c>
       <c r="C54" t="n">
-        <v>4.491243336855411e+228</v>
+        <v>1.049539670704603e+228</v>
       </c>
       <c r="D54" t="n">
-        <v>17.0227823983113</v>
+        <v>0.08091521263122559</v>
       </c>
       <c r="E54" t="n">
-        <v>4.491243336862342e+228</v>
+        <v>121.4191265306944</v>
       </c>
       <c r="F54" t="n">
-        <v>17.0227823983127</v>
+        <v>1.049539670709633e+228</v>
       </c>
       <c r="G54" t="n">
-        <v>4.491243336864141e+228</v>
+        <v>0.01901984214782715</v>
+      </c>
+      <c r="H54" t="n">
+        <v>121.4191265308976</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1.049539670707734e+228</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.0003266334533691406</v>
       </c>
     </row>
     <row r="55">
@@ -1627,22 +2119,31 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>7.080234669429017e-11</v>
+        <v>1.035641040199761e-10</v>
       </c>
       <c r="C55" t="n">
-        <v>6.660356820405203e+233</v>
+        <v>7.593708587441998e+231</v>
       </c>
       <c r="D55" t="n">
-        <v>146.5347297015014</v>
+        <v>0.08685779571533203</v>
       </c>
       <c r="E55" t="n">
-        <v>6.660356820342399e+233</v>
+        <v>235.6434974582012</v>
       </c>
       <c r="F55" t="n">
-        <v>146.5347297013167</v>
+        <v>7.593708588082897e+231</v>
       </c>
       <c r="G55" t="n">
-        <v>6.66035682035578e+233</v>
+        <v>0.02036213874816895</v>
+      </c>
+      <c r="H55" t="n">
+        <v>235.6434974662604</v>
+      </c>
+      <c r="I55" t="n">
+        <v>7.593708587830993e+231</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.0005300045013427734</v>
       </c>
     </row>
     <row r="56">
@@ -1650,22 +2151,31 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>7.166535077721396e-09</v>
+        <v>1.483931103156787e-11</v>
       </c>
       <c r="C56" t="n">
-        <v>2.344919849361154e+237</v>
+        <v>5.500011880671953e+240</v>
       </c>
       <c r="D56" t="n">
-        <v>620.2601963953675</v>
+        <v>0.09018826484680176</v>
       </c>
       <c r="E56" t="n">
-        <v>2.344919850712194e+237</v>
+        <v>10.02868994592199</v>
       </c>
       <c r="F56" t="n">
-        <v>620.2601961743355</v>
+        <v>5.500011880663746e+240</v>
       </c>
       <c r="G56" t="n">
-        <v>2.344919851550355e+237</v>
+        <v>0.02034425735473633</v>
+      </c>
+      <c r="H56" t="n">
+        <v>10.02868994592143</v>
+      </c>
+      <c r="I56" t="n">
+        <v>5.500011880670057e+240</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0003185272216796875</v>
       </c>
     </row>
     <row r="57">
@@ -1673,22 +2183,31 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>7.512849715031723e-11</v>
+        <v>1.326568344176217e-10</v>
       </c>
       <c r="C57" t="n">
-        <v>3.669762785312986e+242</v>
+        <v>1.188202830668417e+244</v>
       </c>
       <c r="D57" t="n">
-        <v>24.31872173933164</v>
+        <v>0.09617519378662109</v>
       </c>
       <c r="E57" t="n">
-        <v>3.669762785312817e+242</v>
+        <v>67.53272854609624</v>
       </c>
       <c r="F57" t="n">
-        <v>24.31872173942183</v>
+        <v>1.188202830703204e+244</v>
       </c>
       <c r="G57" t="n">
-        <v>3.669762785297282e+242</v>
+        <v>0.01782131195068359</v>
+      </c>
+      <c r="H57" t="n">
+        <v>67.53272854779077</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1.188202830673829e+244</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0003950595855712891</v>
       </c>
     </row>
     <row r="58">
@@ -1696,22 +2215,31 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>4.518651392815634e-11</v>
+        <v>1.628981282090554e-10</v>
       </c>
       <c r="C58" t="n">
-        <v>3.78248798967857e+248</v>
+        <v>1.457912223167472e+248</v>
       </c>
       <c r="D58" t="n">
-        <v>13.24116241496745</v>
+        <v>0.1011786460876465</v>
       </c>
       <c r="E58" t="n">
-        <v>3.782487989684518e+248</v>
+        <v>14.72923135778109</v>
       </c>
       <c r="F58" t="n">
-        <v>13.24116241499647</v>
+        <v>1.45791222315702e+248</v>
       </c>
       <c r="G58" t="n">
-        <v>3.782487989673899e+248</v>
+        <v>0.01481080055236816</v>
+      </c>
+      <c r="H58" t="n">
+        <v>14.72923135781446</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1.457912223150358e+248</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.00083160400390625</v>
       </c>
     </row>
     <row r="59">
@@ -1719,22 +2247,31 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>1.667645675060989e-11</v>
+        <v>6.251502061239744e-11</v>
       </c>
       <c r="C59" t="n">
-        <v>3.122452228121564e+254</v>
+        <v>3.166144665723717e+254</v>
       </c>
       <c r="D59" t="n">
-        <v>7.834522007323809</v>
+        <v>0.1043810844421387</v>
       </c>
       <c r="E59" t="n">
-        <v>3.122452228120126e+254</v>
+        <v>9.200823775127873</v>
       </c>
       <c r="F59" t="n">
-        <v>7.83452200732378</v>
+        <v>3.166144665728302e+254</v>
       </c>
       <c r="G59" t="n">
-        <v>3.12245222811962e+254</v>
+        <v>0.01416158676147461</v>
+      </c>
+      <c r="H59" t="n">
+        <v>9.200823775128814</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3.166144665726573e+254</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.0004243850708007812</v>
       </c>
     </row>
     <row r="60">
@@ -1742,22 +2279,31 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>2.852114372232206e-11</v>
+        <v>1.817299364537265e-10</v>
       </c>
       <c r="C60" t="n">
-        <v>6.293267428432717e+259</v>
+        <v>5.534057240407507e+257</v>
       </c>
       <c r="D60" t="n">
-        <v>9.762715619599593</v>
+        <v>0.0988304615020752</v>
       </c>
       <c r="E60" t="n">
-        <v>6.293267428426026e+259</v>
+        <v>9.728171298717761</v>
       </c>
       <c r="F60" t="n">
-        <v>9.762715619595925</v>
+        <v>5.534057240272995e+257</v>
       </c>
       <c r="G60" t="n">
-        <v>6.293267428429115e+259</v>
+        <v>0.01743006706237793</v>
+      </c>
+      <c r="H60" t="n">
+        <v>9.72817129868155</v>
+      </c>
+      <c r="I60" t="n">
+        <v>5.534057240311608e+257</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.002891778945922852</v>
       </c>
     </row>
     <row r="61">
@@ -1765,22 +2311,31 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>1.437107672617035e-10</v>
+        <v>4.057940060769304e-10</v>
       </c>
       <c r="C61" t="n">
-        <v>7.617179594559637e+261</v>
+        <v>6.189966043372978e+259</v>
       </c>
       <c r="D61" t="n">
-        <v>113.5550989352363</v>
+        <v>0.1133708953857422</v>
       </c>
       <c r="E61" t="n">
-        <v>7.61717959444262e+261</v>
+        <v>57.6938252617444</v>
       </c>
       <c r="F61" t="n">
-        <v>113.5550989340993</v>
+        <v>6.189966043407486e+259</v>
       </c>
       <c r="G61" t="n">
-        <v>7.617179594519529e+261</v>
+        <v>0.008632659912109375</v>
+      </c>
+      <c r="H61" t="n">
+        <v>57.69382526167058</v>
+      </c>
+      <c r="I61" t="n">
+        <v>6.189966043445093e+259</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.0004382133483886719</v>
       </c>
     </row>
     <row r="62">
@@ -1788,22 +2343,31 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>4.494476293564833e-09</v>
+        <v>5.279981632262385e-10</v>
       </c>
       <c r="C62" t="n">
-        <v>8.5560645780047e+265</v>
+        <v>1.700120873034899e+263</v>
       </c>
       <c r="D62" t="n">
-        <v>2822.567425950471</v>
+        <v>0.1121630668640137</v>
       </c>
       <c r="E62" t="n">
-        <v>8.55606458063989e+265</v>
+        <v>433.960312674315</v>
       </c>
       <c r="F62" t="n">
-        <v>2822.567425507881</v>
+        <v>1.700120873019066e+263</v>
       </c>
       <c r="G62" t="n">
-        <v>8.556064581983304e+265</v>
+        <v>0.0122833251953125</v>
+      </c>
+      <c r="H62" t="n">
+        <v>433.9603126542453</v>
+      </c>
+      <c r="I62" t="n">
+        <v>1.70012087309185e+263</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.0004208087921142578</v>
       </c>
     </row>
     <row r="63">
@@ -1811,22 +2375,31 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>9.768229453220134e-11</v>
+        <v>3.157155904591938e-11</v>
       </c>
       <c r="C63" t="n">
-        <v>1.082699496056463e+270</v>
+        <v>3.113011685418058e+271</v>
       </c>
       <c r="D63" t="n">
-        <v>37.37446680264031</v>
+        <v>0.1165952682495117</v>
       </c>
       <c r="E63" t="n">
-        <v>1.082699496066704e+270</v>
+        <v>50.87779043753925</v>
       </c>
       <c r="F63" t="n">
-        <v>37.37446680266623</v>
+        <v>3.113011685388426e+271</v>
       </c>
       <c r="G63" t="n">
-        <v>1.082699496067418e+270</v>
+        <v>0.009117364883422852</v>
+      </c>
+      <c r="H63" t="n">
+        <v>50.87779043738066</v>
+      </c>
+      <c r="I63" t="n">
+        <v>3.113011685404813e+271</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.0003809928894042969</v>
       </c>
     </row>
     <row r="64">
@@ -1834,22 +2407,31 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>1.161863201779028e-10</v>
+        <v>7.323796396349604e-11</v>
       </c>
       <c r="C64" t="n">
-        <v>1.37831497768022e+277</v>
+        <v>2.758256390477529e+276</v>
       </c>
       <c r="D64" t="n">
-        <v>107.15562840739</v>
+        <v>0.1228659152984619</v>
       </c>
       <c r="E64" t="n">
-        <v>1.378314977683174e+277</v>
+        <v>28.08868914440245</v>
       </c>
       <c r="F64" t="n">
-        <v>107.1556284081867</v>
+        <v>2.758256390466685e+276</v>
       </c>
       <c r="G64" t="n">
-        <v>1.378314977673711e+277</v>
+        <v>0.01842093467712402</v>
+      </c>
+      <c r="H64" t="n">
+        <v>28.0886891444565</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2.758256390459917e+276</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.003301382064819336</v>
       </c>
     </row>
     <row r="65">
@@ -1857,22 +2439,31 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>1.986540164541516e-11</v>
+        <v>1.638443269434369e-11</v>
       </c>
       <c r="C65" t="n">
-        <v>2.92730546506328e+280</v>
+        <v>1.960730711846066e+280</v>
       </c>
       <c r="D65" t="n">
-        <v>15.80946460937048</v>
+        <v>0.1202895641326904</v>
       </c>
       <c r="E65" t="n">
-        <v>2.927305465058674e+280</v>
+        <v>15.73776832270793</v>
       </c>
       <c r="F65" t="n">
-        <v>15.80946460941645</v>
+        <v>1.960730711834563e+280</v>
       </c>
       <c r="G65" t="n">
-        <v>2.927305465044945e+280</v>
+        <v>0.009759426116943359</v>
+      </c>
+      <c r="H65" t="n">
+        <v>15.73776832269585</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1.960730711836487e+280</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.0004172325134277344</v>
       </c>
     </row>
     <row r="66">
@@ -1880,22 +2471,31 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>9.691893247510797e-12</v>
+        <v>2.723790344005749e-10</v>
       </c>
       <c r="C66" t="n">
-        <v>2.380430954040846e+285</v>
+        <v>2.652049269259207e+286</v>
       </c>
       <c r="D66" t="n">
-        <v>11.34264769981819</v>
+        <v>0.1237945556640625</v>
       </c>
       <c r="E66" t="n">
-        <v>2.380430954036908e+285</v>
+        <v>81.95372824012281</v>
       </c>
       <c r="F66" t="n">
-        <v>11.34264769982059</v>
+        <v>2.652049269235407e+286</v>
       </c>
       <c r="G66" t="n">
-        <v>2.380430954035392e+285</v>
+        <v>0.01140427589416504</v>
+      </c>
+      <c r="H66" t="n">
+        <v>81.95372823990033</v>
+      </c>
+      <c r="I66" t="n">
+        <v>2.652049269244549e+286</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.0004334449768066406</v>
       </c>
     </row>
     <row r="67">
@@ -1903,22 +2503,31 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>9.554440032431527e-12</v>
+        <v>8.258971726921731e-11</v>
       </c>
       <c r="C67" t="n">
-        <v>6.811683699075282e+291</v>
+        <v>3.057827489135899e+290</v>
       </c>
       <c r="D67" t="n">
-        <v>33.67776234346768</v>
+        <v>0.1246926784515381</v>
       </c>
       <c r="E67" t="n">
-        <v>6.811683699052819e+291</v>
+        <v>24.58602251110274</v>
       </c>
       <c r="F67" t="n">
-        <v>33.67776234363598</v>
+        <v>3.057827489139069e+290</v>
       </c>
       <c r="G67" t="n">
-        <v>6.811683699017814e+291</v>
+        <v>0.01016759872436523</v>
+      </c>
+      <c r="H67" t="n">
+        <v>24.58602251107363</v>
+      </c>
+      <c r="I67" t="n">
+        <v>3.05782748914355e+290</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.0003693103790283203</v>
       </c>
     </row>
     <row r="68">
@@ -1926,22 +2535,31 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>6.08105281125106e-09</v>
+        <v>1.173484275211031e-10</v>
       </c>
       <c r="C68" t="n">
-        <v>1.570097687117222e+294</v>
+        <v>1.71252924895886e+294</v>
       </c>
       <c r="D68" t="n">
-        <v>3498.254453041728</v>
+        <v>0.1280815601348877</v>
       </c>
       <c r="E68" t="n">
-        <v>1.570097685495866e+294</v>
+        <v>179.3749359266677</v>
       </c>
       <c r="F68" t="n">
-        <v>3498.254448426049</v>
+        <v>1.712529248950993e+294</v>
       </c>
       <c r="G68" t="n">
-        <v>1.570097687564034e+294</v>
+        <v>0.01177024841308594</v>
+      </c>
+      <c r="H68" t="n">
+        <v>179.3749359270734</v>
+      </c>
+      <c r="I68" t="n">
+        <v>1.712529248949956e+294</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.0004107952117919922</v>
       </c>
     </row>
     <row r="69">
@@ -1949,22 +2567,31 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>1.21598533325218e-07</v>
+        <v>4.97287819328355e-11</v>
       </c>
       <c r="C69" t="n">
-        <v>2.560329492689976e+296</v>
+        <v>5.708479779142257e+299</v>
       </c>
       <c r="D69" t="n">
-        <v>59531.69552711697</v>
+        <v>0.1289312839508057</v>
       </c>
       <c r="E69" t="n">
-        <v>2.560329514264868e+296</v>
+        <v>29.50369576382774</v>
       </c>
       <c r="F69" t="n">
-        <v>59531.69631354768</v>
+        <v>5.708479779157505e+299</v>
       </c>
       <c r="G69" t="n">
-        <v>2.560329480440644e+296</v>
+        <v>0.0109550952911377</v>
+      </c>
+      <c r="H69" t="n">
+        <v>29.50369576387726</v>
+      </c>
+      <c r="I69" t="n">
+        <v>5.708479779131563e+299</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.0003755092620849609</v>
       </c>
     </row>
     <row r="70">
@@ -1972,22 +2599,31 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>7.647176442686957e-11</v>
+        <v>6.746869671983728e-11</v>
       </c>
       <c r="C70" t="n">
-        <v>2.050881651296044e+304</v>
+        <v>1.060013809202805e+304</v>
       </c>
       <c r="D70" t="n">
-        <v>67.77072478056168</v>
+        <v>0.1338894367218018</v>
       </c>
       <c r="E70" t="n">
-        <v>2.050881651299559e+304</v>
+        <v>63.35975391480676</v>
       </c>
       <c r="F70" t="n">
-        <v>67.77072478059522</v>
+        <v>1.060013809210319e+304</v>
       </c>
       <c r="G70" t="n">
-        <v>2.050881651298464e+304</v>
+        <v>0.01202702522277832</v>
+      </c>
+      <c r="H70" t="n">
+        <v>63.35975391496337</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1.060013809206765e+304</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.0004761219024658203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcao de alguns erros no programa T1 e adicao de diretorio com metodos iterativos
</commit_message>
<xml_diff>
--- a/T1/resultados_Cholesky.xlsx
+++ b/T1/resultados_Cholesky.xlsx
@@ -423,31 +423,31 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3.14018491736755e-16</v>
       </c>
       <c r="C2" t="n">
-        <v>811801.0000000006</v>
+        <v>11930116</v>
       </c>
       <c r="D2" t="n">
-        <v>6.985664367675781e-05</v>
+        <v>0.0002412796020507812</v>
       </c>
       <c r="E2" t="n">
-        <v>1.606934272667016</v>
+        <v>1.400333477469933</v>
       </c>
       <c r="F2" t="n">
-        <v>811800.999999998</v>
+        <v>11930116</v>
       </c>
       <c r="G2" t="n">
-        <v>2.932548522949219e-05</v>
+        <v>9.512901306152344e-05</v>
       </c>
       <c r="H2" t="n">
-        <v>1.606934272667016</v>
+        <v>1.400333477469933</v>
       </c>
       <c r="I2" t="n">
-        <v>811800.9999999981</v>
+        <v>11930116</v>
       </c>
       <c r="J2" t="n">
-        <v>5.769729614257812e-05</v>
+        <v>0.0001730918884277344</v>
       </c>
     </row>
     <row r="3">
@@ -455,31 +455,31 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>8.000541662143798e-15</v>
+        <v>3.33066907387547e-16</v>
       </c>
       <c r="C3" t="n">
-        <v>12449426929.00007</v>
+        <v>119221731225</v>
       </c>
       <c r="D3" t="n">
-        <v>7.891654968261719e-05</v>
+        <v>0.0002684593200683594</v>
       </c>
       <c r="E3" t="n">
-        <v>1.707792150386513</v>
+        <v>1.69784411252049</v>
       </c>
       <c r="F3" t="n">
-        <v>12449426929.00001</v>
+        <v>119221731225</v>
       </c>
       <c r="G3" t="n">
-        <v>3.910064697265625e-05</v>
+        <v>0.0001301765441894531</v>
       </c>
       <c r="H3" t="n">
-        <v>1.707792150386513</v>
+        <v>1.69784411252049</v>
       </c>
       <c r="I3" t="n">
-        <v>12449426928.99998</v>
+        <v>119221731225.0001</v>
       </c>
       <c r="J3" t="n">
-        <v>3.910064697265625e-05</v>
+        <v>0.0001180171966552734</v>
       </c>
     </row>
     <row r="4">
@@ -487,31 +487,31 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.499598997848221e-13</v>
+        <v>2.369747574962801e-14</v>
       </c>
       <c r="C4" t="n">
-        <v>3642505846225.029</v>
+        <v>74089641561155.81</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001087188720703125</v>
+        <v>0.000370025634765625</v>
       </c>
       <c r="E4" t="n">
-        <v>9.22858758939134</v>
+        <v>2.010189784364854</v>
       </c>
       <c r="F4" t="n">
-        <v>3642505846224.929</v>
+        <v>74089641561155.94</v>
       </c>
       <c r="G4" t="n">
-        <v>5.91278076171875e-05</v>
+        <v>0.0002667903900146484</v>
       </c>
       <c r="H4" t="n">
-        <v>9.228587589391163</v>
+        <v>2.010189784364854</v>
       </c>
       <c r="I4" t="n">
-        <v>3642505846224.987</v>
+        <v>74089641561155.67</v>
       </c>
       <c r="J4" t="n">
-        <v>3.4332275390625e-05</v>
+        <v>0.0001261234283447266</v>
       </c>
     </row>
     <row r="5">
@@ -519,31 +519,31 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.855027013458529e-10</v>
+        <v>6.156324321644999e-14</v>
       </c>
       <c r="C5" t="n">
-        <v>37239773954134.3</v>
+        <v>1.104981964730335e+17</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0001480579376220703</v>
+        <v>0.0004966259002685547</v>
       </c>
       <c r="E5" t="n">
-        <v>951.6137504317491</v>
+        <v>2.331907935311975</v>
       </c>
       <c r="F5" t="n">
-        <v>37239773953438.41</v>
+        <v>1.104981964730378e+17</v>
       </c>
       <c r="G5" t="n">
-        <v>8.368492126464844e-05</v>
+        <v>0.0002737045288085938</v>
       </c>
       <c r="H5" t="n">
-        <v>951.6137504139588</v>
+        <v>2.331907935311979</v>
       </c>
       <c r="I5" t="n">
-        <v>37239773954134.29</v>
+        <v>1.104981964730353e+17</v>
       </c>
       <c r="J5" t="n">
-        <v>3.457069396972656e-05</v>
+        <v>0.0001215934753417969</v>
       </c>
     </row>
     <row r="6">
@@ -551,31 +551,31 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>1.778922377480441e-14</v>
+        <v>2.452557043703863e-13</v>
       </c>
       <c r="C6" t="n">
-        <v>2.518612275825941e+21</v>
+        <v>2.713477193275128e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001931190490722656</v>
+        <v>0.0006656646728515625</v>
       </c>
       <c r="E6" t="n">
-        <v>2.435596948390076</v>
+        <v>2.860380046727197</v>
       </c>
       <c r="F6" t="n">
-        <v>2.518612275825948e+21</v>
+        <v>2.713477193274867e+18</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0001099109649658203</v>
+        <v>0.0003843307495117188</v>
       </c>
       <c r="H6" t="n">
-        <v>2.435596948390075</v>
+        <v>2.860380046727198</v>
       </c>
       <c r="I6" t="n">
-        <v>2.51861227582595e+21</v>
+        <v>2.713477193274862e+18</v>
       </c>
       <c r="J6" t="n">
-        <v>3.504753112792969e-05</v>
+        <v>0.0001430511474609375</v>
       </c>
     </row>
     <row r="7">
@@ -583,31 +583,31 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>2.621137574964887e-14</v>
+        <v>1.832645318255899e-13</v>
       </c>
       <c r="C7" t="n">
-        <v>5.129658090748854e+25</v>
+        <v>1.161712635273819e+25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000247955322265625</v>
+        <v>0.0009987354278564453</v>
       </c>
       <c r="E7" t="n">
-        <v>2.594806261506959</v>
+        <v>3.226733327967174</v>
       </c>
       <c r="F7" t="n">
-        <v>5.129658090748897e+25</v>
+        <v>1.16171263527382e+25</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0001435279846191406</v>
+        <v>0.0004854202270507812</v>
       </c>
       <c r="H7" t="n">
-        <v>2.59480626150696</v>
+        <v>3.226733327967167</v>
       </c>
       <c r="I7" t="n">
-        <v>5.129658090748888e+25</v>
+        <v>1.161712635273826e+25</v>
       </c>
       <c r="J7" t="n">
-        <v>3.647804260253906e-05</v>
+        <v>0.0001506805419921875</v>
       </c>
     </row>
     <row r="8">
@@ -615,31 +615,31 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1.045733441113283e-14</v>
+        <v>3.28839738738339e-14</v>
       </c>
       <c r="C8" t="n">
-        <v>8.568046341833192e+27</v>
+        <v>2.345743096656882e+28</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0003144741058349609</v>
+        <v>0.00108790397644043</v>
       </c>
       <c r="E8" t="n">
-        <v>2.793486383530426</v>
+        <v>2.984379207132995</v>
       </c>
       <c r="F8" t="n">
-        <v>8.568046341833138e+27</v>
+        <v>2.345743096656904e+28</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001783370971679688</v>
+        <v>0.0006103515625</v>
       </c>
       <c r="H8" t="n">
-        <v>2.793486383530426</v>
+        <v>2.984379207132995</v>
       </c>
       <c r="I8" t="n">
-        <v>8.568046341833212e+27</v>
+        <v>2.345743096656893e+28</v>
       </c>
       <c r="J8" t="n">
-        <v>3.957748413085938e-05</v>
+        <v>0.0001769065856933594</v>
       </c>
     </row>
     <row r="9">
@@ -647,31 +647,31 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>3.523461519555973e-13</v>
+        <v>1.35996361066808e-11</v>
       </c>
       <c r="C9" t="n">
-        <v>2.679576537875895e+31</v>
+        <v>9.352974121082972e+28</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0003848075866699219</v>
+        <v>0.002604007720947266</v>
       </c>
       <c r="E9" t="n">
-        <v>17.98858265091783</v>
+        <v>239.0921145815003</v>
       </c>
       <c r="F9" t="n">
-        <v>2.679576537876005e+31</v>
+        <v>9.352974121101077e+28</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0002229213714599609</v>
+        <v>0.001476287841796875</v>
       </c>
       <c r="H9" t="n">
-        <v>17.98858265092075</v>
+        <v>239.0921145811405</v>
       </c>
       <c r="I9" t="n">
-        <v>2.679576537875533e+31</v>
+        <v>9.352974121115017e+28</v>
       </c>
       <c r="J9" t="n">
-        <v>3.695487976074219e-05</v>
+        <v>0.0002624988555908203</v>
       </c>
     </row>
     <row r="10">
@@ -679,31 +679,31 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>5.439579601525954e-13</v>
+        <v>1.847638281064545e-13</v>
       </c>
       <c r="C10" t="n">
-        <v>8.073525320320142e+35</v>
+        <v>3.566691517516605e+35</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0004799365997314453</v>
+        <v>0.003186941146850586</v>
       </c>
       <c r="E10" t="n">
-        <v>4.089790696438899</v>
+        <v>3.196565922500234</v>
       </c>
       <c r="F10" t="n">
-        <v>8.073525320321085e+35</v>
+        <v>3.56669151751654e+35</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002725124359130859</v>
+        <v>0.001131534576416016</v>
       </c>
       <c r="H10" t="n">
-        <v>4.089790696438723</v>
+        <v>3.196565922500233</v>
       </c>
       <c r="I10" t="n">
-        <v>8.07352532032183e+35</v>
+        <v>3.566691517516446e+35</v>
       </c>
       <c r="J10" t="n">
-        <v>4.911422729492188e-05</v>
+        <v>0.0001785755157470703</v>
       </c>
     </row>
     <row r="11">
@@ -711,31 +711,31 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>1.189849505328036e-12</v>
+        <v>6.252541798092533e-11</v>
       </c>
       <c r="C11" t="n">
-        <v>4.171031611536207e+39</v>
+        <v>4.333708633854715e+38</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0006587505340576172</v>
+        <v>0.001941204071044922</v>
       </c>
       <c r="E11" t="n">
-        <v>17.35729338441737</v>
+        <v>44.69094411805312</v>
       </c>
       <c r="F11" t="n">
-        <v>4.171031611535826e+39</v>
+        <v>4.333708633846468e+38</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0003352165222167969</v>
+        <v>0.001087188720703125</v>
       </c>
       <c r="H11" t="n">
-        <v>17.35729338443337</v>
+        <v>44.69094411808447</v>
       </c>
       <c r="I11" t="n">
-        <v>4.171031611531885e+39</v>
+        <v>4.3337086338434e+38</v>
       </c>
       <c r="J11" t="n">
-        <v>9.918212890625e-05</v>
+        <v>0.0002195835113525391</v>
       </c>
     </row>
     <row r="12">
@@ -743,31 +743,31 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>1.800188887067328e-11</v>
+        <v>4.569929623769366e-13</v>
       </c>
       <c r="C12" t="n">
-        <v>3.75768503856845e+42</v>
+        <v>3.254448108835348e+44</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001394748687744141</v>
+        <v>0.002439975738525391</v>
       </c>
       <c r="E12" t="n">
-        <v>24.23806724851069</v>
+        <v>3.63363303703942</v>
       </c>
       <c r="F12" t="n">
-        <v>3.757685038571573e+42</v>
+        <v>3.254448108834866e+44</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0007874965667724609</v>
+        <v>0.001286983489990234</v>
       </c>
       <c r="H12" t="n">
-        <v>24.23806724839061</v>
+        <v>3.633633037039418</v>
       </c>
       <c r="I12" t="n">
-        <v>3.757685038589905e+42</v>
+        <v>3.254448108835245e+44</v>
       </c>
       <c r="J12" t="n">
-        <v>0.00011444091796875</v>
+        <v>0.0001587867736816406</v>
       </c>
     </row>
     <row r="13">
@@ -775,31 +775,31 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>3.4837544270714e-13</v>
+        <v>3.395258798382799e-11</v>
       </c>
       <c r="C13" t="n">
-        <v>1.094466987402113e+47</v>
+        <v>1.130992291042399e+46</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0008699893951416016</v>
+        <v>0.002829790115356445</v>
       </c>
       <c r="E13" t="n">
-        <v>5.648290483218029</v>
+        <v>91.5437501854671</v>
       </c>
       <c r="F13" t="n">
-        <v>1.094466987402478e+47</v>
+        <v>1.130992291041235e+46</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0004897117614746094</v>
+        <v>0.001499652862548828</v>
       </c>
       <c r="H13" t="n">
-        <v>5.6482904832174</v>
+        <v>91.5437501853775</v>
       </c>
       <c r="I13" t="n">
-        <v>1.094466987402749e+47</v>
+        <v>1.1309922910424e+46</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0001423358917236328</v>
+        <v>0.0001494884490966797</v>
       </c>
     </row>
     <row r="14">
@@ -807,31 +807,31 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>8.201347561477511e-14</v>
+        <v>2.863230741432622e-13</v>
       </c>
       <c r="C14" t="n">
-        <v>7.203368753278922e+54</v>
+        <v>3.750508721117903e+51</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0009775161743164062</v>
+        <v>0.003247261047363281</v>
       </c>
       <c r="E14" t="n">
-        <v>3.745807663783038</v>
+        <v>3.861377208438245</v>
       </c>
       <c r="F14" t="n">
-        <v>7.203368753278949e+54</v>
+        <v>3.750508721118136e+51</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000522613525390625</v>
+        <v>0.001729488372802734</v>
       </c>
       <c r="H14" t="n">
-        <v>3.745807663783038</v>
+        <v>3.861377208438217</v>
       </c>
       <c r="I14" t="n">
-        <v>7.203368753279021e+54</v>
+        <v>3.750508721118586e+51</v>
       </c>
       <c r="J14" t="n">
-        <v>5.960464477539062e-05</v>
+        <v>0.0001533031463623047</v>
       </c>
     </row>
     <row r="15">
@@ -839,31 +839,31 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>1.036637232883434e-09</v>
+        <v>2.482970047976386e-13</v>
       </c>
       <c r="C15" t="n">
-        <v>6.40347104687479e+53</v>
+        <v>1.347432847557717e+57</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001154661178588867</v>
+        <v>0.003867864608764648</v>
       </c>
       <c r="E15" t="n">
-        <v>4246.598294734663</v>
+        <v>3.990014873321611</v>
       </c>
       <c r="F15" t="n">
-        <v>6.403471047114816e+53</v>
+        <v>1.347432847557682e+57</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0005393028259277344</v>
+        <v>0.001995086669921875</v>
       </c>
       <c r="H15" t="n">
-        <v>4246.598293908219</v>
+        <v>3.990014873321607</v>
       </c>
       <c r="I15" t="n">
-        <v>6.403471048360951e+53</v>
+        <v>1.347432847557704e+57</v>
       </c>
       <c r="J15" t="n">
-        <v>5.388259887695312e-05</v>
+        <v>0.0001583099365234375</v>
       </c>
     </row>
     <row r="16">
@@ -871,31 +871,31 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>2.31370685832686e-12</v>
+        <v>9.071511609732763e-13</v>
       </c>
       <c r="C16" t="n">
-        <v>7.83098495134326e+60</v>
+        <v>1.046261505869148e+60</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001305341720581055</v>
+        <v>0.004471778869628906</v>
       </c>
       <c r="E16" t="n">
-        <v>63.08899475504415</v>
+        <v>4.343342844367386</v>
       </c>
       <c r="F16" t="n">
-        <v>7.830984951345365e+60</v>
+        <v>1.04626150586888e+60</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0005953311920166016</v>
+        <v>0.003511190414428711</v>
       </c>
       <c r="H16" t="n">
-        <v>63.08899475506855</v>
+        <v>4.343342844367421</v>
       </c>
       <c r="I16" t="n">
-        <v>7.830984951342824e+60</v>
+        <v>1.046261505868866e+60</v>
       </c>
       <c r="J16" t="n">
-        <v>5.507469177246094e-05</v>
+        <v>0.0002839565277099609</v>
       </c>
     </row>
     <row r="17">
@@ -903,31 +903,31 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>2.046263628128219e-12</v>
+        <v>8.230496124954359e-10</v>
       </c>
       <c r="C17" t="n">
-        <v>7.774210352096991e+62</v>
+        <v>8.35893904575978e+60</v>
       </c>
       <c r="D17" t="n">
-        <v>0.001547098159790039</v>
+        <v>0.005321979522705078</v>
       </c>
       <c r="E17" t="n">
-        <v>8.278012055997321</v>
+        <v>16823.54821205804</v>
       </c>
       <c r="F17" t="n">
-        <v>7.774210352093635e+62</v>
+        <v>8.358939046652196e+60</v>
       </c>
       <c r="G17" t="n">
-        <v>0.000667572021484375</v>
+        <v>0.002494335174560547</v>
       </c>
       <c r="H17" t="n">
-        <v>8.278012055995735</v>
+        <v>16823.54821061932</v>
       </c>
       <c r="I17" t="n">
-        <v>7.774210352097547e+62</v>
+        <v>8.358939047366981e+60</v>
       </c>
       <c r="J17" t="n">
-        <v>5.793571472167969e-05</v>
+        <v>0.0001778602600097656</v>
       </c>
     </row>
     <row r="18">
@@ -935,31 +935,31 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>1.358096973651833e-10</v>
+        <v>1.297567333377152e-11</v>
       </c>
       <c r="C18" t="n">
-        <v>2.003483347477747e+67</v>
+        <v>1.906404039012632e+66</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004569768905639648</v>
+        <v>0.01509237289428711</v>
       </c>
       <c r="E18" t="n">
-        <v>6.5975934225286</v>
+        <v>59.45467037571392</v>
       </c>
       <c r="F18" t="n">
-        <v>2.003483347474869e+67</v>
+        <v>1.906404039011311e+66</v>
       </c>
       <c r="G18" t="n">
-        <v>0.002137660980224609</v>
+        <v>0.007136106491088867</v>
       </c>
       <c r="H18" t="n">
-        <v>6.597593422530255</v>
+        <v>59.45467037567589</v>
       </c>
       <c r="I18" t="n">
-        <v>2.003483347474182e+67</v>
+        <v>1.906404039012722e+66</v>
       </c>
       <c r="J18" t="n">
-        <v>0.000125885009765625</v>
+        <v>0.0004091262817382812</v>
       </c>
     </row>
     <row r="19">
@@ -967,31 +967,31 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>1.013967363057377e-13</v>
+        <v>2.75723056447094e-12</v>
       </c>
       <c r="C19" t="n">
-        <v>2.750689858298729e+74</v>
+        <v>7.034778490781662e+73</v>
       </c>
       <c r="D19" t="n">
-        <v>0.005156755447387695</v>
+        <v>0.01714944839477539</v>
       </c>
       <c r="E19" t="n">
-        <v>4.361995134102214</v>
+        <v>6.629216560315689</v>
       </c>
       <c r="F19" t="n">
-        <v>2.750689858298881e+74</v>
+        <v>7.034778490779204e+73</v>
       </c>
       <c r="G19" t="n">
-        <v>0.002362489700317383</v>
+        <v>0.007974147796630859</v>
       </c>
       <c r="H19" t="n">
-        <v>4.361995134102216</v>
+        <v>6.629216560315963</v>
       </c>
       <c r="I19" t="n">
-        <v>2.750689858298686e+74</v>
+        <v>7.034778490778587e+73</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0001251697540283203</v>
+        <v>0.0004193782806396484</v>
       </c>
     </row>
     <row r="20">
@@ -999,31 +999,31 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>2.76733680660669e-10</v>
+        <v>2.615149146059597e-11</v>
       </c>
       <c r="C20" t="n">
-        <v>4.808210008653512e+74</v>
+        <v>2.861536195854224e+76</v>
       </c>
       <c r="D20" t="n">
-        <v>0.005887746810913086</v>
+        <v>0.01974058151245117</v>
       </c>
       <c r="E20" t="n">
-        <v>91.5023845242263</v>
+        <v>478.4723397227564</v>
       </c>
       <c r="F20" t="n">
-        <v>4.808210008409245e+74</v>
+        <v>2.861536195910177e+76</v>
       </c>
       <c r="G20" t="n">
-        <v>0.002637386322021484</v>
+        <v>0.008874893188476562</v>
       </c>
       <c r="H20" t="n">
-        <v>91.50238452309671</v>
+        <v>478.4723397177511</v>
       </c>
       <c r="I20" t="n">
-        <v>4.808210008468947e+74</v>
+        <v>2.861536195940136e+76</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0001366138458251953</v>
+        <v>0.000408172607421875</v>
       </c>
     </row>
     <row r="21">
@@ -1031,31 +1031,31 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>6.054627505789501e-11</v>
+        <v>9.688736131304309e-13</v>
       </c>
       <c r="C21" t="n">
-        <v>1.297052066748948e+81</v>
+        <v>3.340838350510316e+81</v>
       </c>
       <c r="D21" t="n">
-        <v>0.006605625152587891</v>
+        <v>0.0222010612487793</v>
       </c>
       <c r="E21" t="n">
-        <v>150.864593763022</v>
+        <v>5.50089107213675</v>
       </c>
       <c r="F21" t="n">
-        <v>1.29705206674521e+81</v>
+        <v>3.340838350511341e+81</v>
       </c>
       <c r="G21" t="n">
-        <v>0.002880573272705078</v>
+        <v>0.009908437728881836</v>
       </c>
       <c r="H21" t="n">
-        <v>150.8645937634588</v>
+        <v>5.500891072136812</v>
       </c>
       <c r="I21" t="n">
-        <v>1.297052066741504e+81</v>
+        <v>3.340838350511048e+81</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0001306533813476562</v>
+        <v>0.0004320144653320312</v>
       </c>
     </row>
     <row r="22">
@@ -1063,31 +1063,31 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>1.880886477037752e-10</v>
+        <v>1.509162606315114e-11</v>
       </c>
       <c r="C22" t="n">
-        <v>3.744272979213227e+83</v>
+        <v>4.677437921399251e+83</v>
       </c>
       <c r="D22" t="n">
-        <v>0.007464408874511719</v>
+        <v>0.02487802505493164</v>
       </c>
       <c r="E22" t="n">
-        <v>535.8838690149026</v>
+        <v>37.50305690971421</v>
       </c>
       <c r="F22" t="n">
-        <v>3.744272979043216e+83</v>
+        <v>4.677437921404781e+83</v>
       </c>
       <c r="G22" t="n">
-        <v>0.003165721893310547</v>
+        <v>0.01058697700500488</v>
       </c>
       <c r="H22" t="n">
-        <v>535.883869031986</v>
+        <v>37.50305690969743</v>
       </c>
       <c r="I22" t="n">
-        <v>3.744272978924728e+83</v>
+        <v>4.677437921408532e+83</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0001320838928222656</v>
+        <v>0.0004322528839111328</v>
       </c>
     </row>
     <row r="23">
@@ -1095,31 +1095,31 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>1.825891293297175e-12</v>
+        <v>2.092249232586236e-12</v>
       </c>
       <c r="C23" t="n">
-        <v>1.45028900949697e+92</v>
+        <v>9.187390591271938e+90</v>
       </c>
       <c r="D23" t="n">
-        <v>0.008332967758178711</v>
+        <v>0.02766752243041992</v>
       </c>
       <c r="E23" t="n">
-        <v>4.784842078780625</v>
+        <v>5.524603424217057</v>
       </c>
       <c r="F23" t="n">
-        <v>1.450289009497246e+92</v>
+        <v>9.187390591271596e+90</v>
       </c>
       <c r="G23" t="n">
-        <v>0.003452301025390625</v>
+        <v>0.01194643974304199</v>
       </c>
       <c r="H23" t="n">
-        <v>4.784842078780625</v>
+        <v>5.524603424217132</v>
       </c>
       <c r="I23" t="n">
-        <v>1.450289009497316e+92</v>
+        <v>9.18739059127194e+90</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0001409053802490234</v>
+        <v>0.0004909038543701172</v>
       </c>
     </row>
     <row r="24">
@@ -1127,31 +1127,31 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>1.135907499779978e-10</v>
+        <v>2.35753750753081e-11</v>
       </c>
       <c r="C24" t="n">
-        <v>2.279646083948241e+93</v>
+        <v>4.62930137435475e+93</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00938725471496582</v>
+        <v>0.03088164329528809</v>
       </c>
       <c r="E24" t="n">
-        <v>155.3058689827857</v>
+        <v>36.94040816057532</v>
       </c>
       <c r="F24" t="n">
-        <v>2.27964608399781e+93</v>
+        <v>4.629301374325221e+93</v>
       </c>
       <c r="G24" t="n">
-        <v>0.003787040710449219</v>
+        <v>0.01265597343444824</v>
       </c>
       <c r="H24" t="n">
-        <v>155.3058689851258</v>
+        <v>36.94040816043792</v>
       </c>
       <c r="I24" t="n">
-        <v>2.279646083963636e+93</v>
+        <v>4.629301374342827e+93</v>
       </c>
       <c r="J24" t="n">
-        <v>0.002804994583129883</v>
+        <v>0.0004239082336425781</v>
       </c>
     </row>
     <row r="25">
@@ -1159,31 +1159,31 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>2.834646218533476e-12</v>
+        <v>3.237860676215449e-10</v>
       </c>
       <c r="C25" t="n">
-        <v>1.328058644082522e+97</v>
+        <v>5.703804416368528e+95</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01133489608764648</v>
+        <v>0.03286027908325195</v>
       </c>
       <c r="E25" t="n">
-        <v>5.379997973112778</v>
+        <v>401.6583184370128</v>
       </c>
       <c r="F25" t="n">
-        <v>1.328058644084436e+97</v>
+        <v>5.703804416352753e+95</v>
       </c>
       <c r="G25" t="n">
-        <v>0.004102468490600586</v>
+        <v>0.01367568969726562</v>
       </c>
       <c r="H25" t="n">
-        <v>5.379997973112701</v>
+        <v>401.658318436124</v>
       </c>
       <c r="I25" t="n">
-        <v>1.32805864408419e+97</v>
+        <v>5.703804416365568e+95</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0001993179321289062</v>
+        <v>0.0004990100860595703</v>
       </c>
     </row>
     <row r="26">
@@ -1191,31 +1191,31 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>3.123899317305387e-12</v>
+        <v>1.030229827065441e-12</v>
       </c>
       <c r="C26" t="n">
-        <v>3.250023257561461e+102</v>
+        <v>6.941396556156472e+104</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01136159896850586</v>
+        <v>0.0389096736907959</v>
       </c>
       <c r="E26" t="n">
-        <v>5.250576972835259</v>
+        <v>5.189324674177794</v>
       </c>
       <c r="F26" t="n">
-        <v>3.250023257560635e+102</v>
+        <v>6.94139655615492e+104</v>
       </c>
       <c r="G26" t="n">
-        <v>0.004439115524291992</v>
+        <v>0.01483345031738281</v>
       </c>
       <c r="H26" t="n">
-        <v>5.250576972835288</v>
+        <v>5.189324674177792</v>
       </c>
       <c r="I26" t="n">
-        <v>3.250023257560464e+102</v>
+        <v>6.941396556155032e+104</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0001566410064697266</v>
+        <v>0.0004923343658447266</v>
       </c>
     </row>
     <row r="27">
@@ -1223,31 +1223,31 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>5.287360592543865e-12</v>
+        <v>4.709653202008775e-12</v>
       </c>
       <c r="C27" t="n">
-        <v>2.040042359044407e+107</v>
+        <v>8.243519749463029e+107</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0126805305480957</v>
+        <v>0.04267191886901855</v>
       </c>
       <c r="E27" t="n">
-        <v>8.796535256700455</v>
+        <v>9.015680508915349</v>
       </c>
       <c r="F27" t="n">
-        <v>2.040042359042814e+107</v>
+        <v>8.243519749465098e+107</v>
       </c>
       <c r="G27" t="n">
-        <v>0.004745721817016602</v>
+        <v>0.01602029800415039</v>
       </c>
       <c r="H27" t="n">
-        <v>8.796535256691179</v>
+        <v>9.015680508917105</v>
       </c>
       <c r="I27" t="n">
-        <v>2.040042359045911e+107</v>
+        <v>8.243519749464033e+107</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0001780986785888672</v>
+        <v>0.0006175041198730469</v>
       </c>
     </row>
     <row r="28">
@@ -1255,31 +1255,31 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>1.653541930717623e-11</v>
+        <v>4.839504666288376e-11</v>
       </c>
       <c r="C28" t="n">
-        <v>4.797403182337988e+111</v>
+        <v>7.76276851853745e+109</v>
       </c>
       <c r="D28" t="n">
-        <v>0.01381874084472656</v>
+        <v>0.04591679573059082</v>
       </c>
       <c r="E28" t="n">
-        <v>12.46357414067869</v>
+        <v>149.6101935479357</v>
       </c>
       <c r="F28" t="n">
-        <v>4.797403182338475e+111</v>
+        <v>7.762768518495119e+109</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00510716438293457</v>
+        <v>0.01709675788879395</v>
       </c>
       <c r="H28" t="n">
-        <v>12.46357414068513</v>
+        <v>149.610193547735</v>
       </c>
       <c r="I28" t="n">
-        <v>4.797403182335759e+111</v>
+        <v>7.762768518506024e+109</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0001828670501708984</v>
+        <v>0.0004980564117431641</v>
       </c>
     </row>
     <row r="29">
@@ -1287,31 +1287,31 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>2.309711318461324e-12</v>
+        <v>9.773388252704239e-13</v>
       </c>
       <c r="C29" t="n">
-        <v>1.676771441443842e+118</v>
+        <v>1.142837886612337e+117</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01521706581115723</v>
+        <v>0.05027604103088379</v>
       </c>
       <c r="E29" t="n">
-        <v>5.769081349457414</v>
+        <v>5.66070615558209</v>
       </c>
       <c r="F29" t="n">
-        <v>1.676771441444299e+118</v>
+        <v>1.142837886611769e+117</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00548100471496582</v>
+        <v>0.01848816871643066</v>
       </c>
       <c r="H29" t="n">
-        <v>5.769081349457416</v>
+        <v>5.660706155582123</v>
       </c>
       <c r="I29" t="n">
-        <v>1.676771441444281e+118</v>
+        <v>1.142837886611816e+117</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0001688003540039062</v>
+        <v>0.0005617141723632812</v>
       </c>
     </row>
     <row r="30">
@@ -1319,31 +1319,31 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>1.351245301341664e-10</v>
+        <v>9.434659063244193e-13</v>
       </c>
       <c r="C30" t="n">
-        <v>9.96983613809841e+118</v>
+        <v>3.84351454282058e+120</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01657605171203613</v>
+        <v>0.05483508110046387</v>
       </c>
       <c r="E30" t="n">
-        <v>235.2558803922626</v>
+        <v>25.10949127983783</v>
       </c>
       <c r="F30" t="n">
-        <v>9.969836139481465e+118</v>
+        <v>3.843514542820603e+120</v>
       </c>
       <c r="G30" t="n">
-        <v>0.005850553512573242</v>
+        <v>0.0197446346282959</v>
       </c>
       <c r="H30" t="n">
-        <v>235.2558804016487</v>
+        <v>25.10949127984163</v>
       </c>
       <c r="I30" t="n">
-        <v>9.969836139085113e+118</v>
+        <v>3.843514542819969e+120</v>
       </c>
       <c r="J30" t="n">
-        <v>0.0001819133758544922</v>
+        <v>0.0005621910095214844</v>
       </c>
     </row>
     <row r="31">
@@ -1351,31 +1351,31 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>1.130925235834915e-10</v>
+        <v>2.4257373301672e-10</v>
       </c>
       <c r="C31" t="n">
-        <v>1.020613207155643e+121</v>
+        <v>2.794654498504583e+121</v>
       </c>
       <c r="D31" t="n">
-        <v>0.01802945137023926</v>
+        <v>0.06046152114868164</v>
       </c>
       <c r="E31" t="n">
-        <v>1007.587675735851</v>
+        <v>134.5381118186002</v>
       </c>
       <c r="F31" t="n">
-        <v>1.020613207126407e+121</v>
+        <v>2.794654498580943e+121</v>
       </c>
       <c r="G31" t="n">
-        <v>0.006236553192138672</v>
+        <v>0.02108955383300781</v>
       </c>
       <c r="H31" t="n">
-        <v>1007.587675749527</v>
+        <v>134.5381118173464</v>
       </c>
       <c r="I31" t="n">
-        <v>1.020613207112371e+121</v>
+        <v>2.794654498610423e+121</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0002124309539794922</v>
+        <v>0.0007255077362060547</v>
       </c>
     </row>
     <row r="32">
@@ -1383,31 +1383,31 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>6.37898313335823e-12</v>
+        <v>5.643538293615139e-11</v>
       </c>
       <c r="C32" t="n">
-        <v>1.403452518247407e+129</v>
+        <v>2.027726880409896e+128</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01980781555175781</v>
+        <v>0.06536364555358887</v>
       </c>
       <c r="E32" t="n">
-        <v>11.56887242829396</v>
+        <v>46.58016088187594</v>
       </c>
       <c r="F32" t="n">
-        <v>1.40345251824679e+129</v>
+        <v>2.027726880408706e+128</v>
       </c>
       <c r="G32" t="n">
-        <v>0.006657600402832031</v>
+        <v>0.02225923538208008</v>
       </c>
       <c r="H32" t="n">
-        <v>11.56887242829289</v>
+        <v>46.58016088186613</v>
       </c>
       <c r="I32" t="n">
-        <v>1.403452518246926e+129</v>
+        <v>2.027726880408635e+128</v>
       </c>
       <c r="J32" t="n">
-        <v>0.0002241134643554688</v>
+        <v>0.0006940364837646484</v>
       </c>
     </row>
     <row r="33">
@@ -1415,31 +1415,31 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>5.681038297748872e-12</v>
+        <v>1.076733073064645e-11</v>
       </c>
       <c r="C33" t="n">
-        <v>1.187162776348539e+134</v>
+        <v>2.137831351624331e+133</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02129507064819336</v>
+        <v>0.07089948654174805</v>
       </c>
       <c r="E33" t="n">
-        <v>10.02571269005637</v>
+        <v>7.64899948286603</v>
       </c>
       <c r="F33" t="n">
-        <v>1.187162776348602e+134</v>
+        <v>2.137831351623527e+133</v>
       </c>
       <c r="G33" t="n">
-        <v>0.007094144821166992</v>
+        <v>0.02391457557678223</v>
       </c>
       <c r="H33" t="n">
-        <v>10.02571269005756</v>
+        <v>7.648999482865413</v>
       </c>
       <c r="I33" t="n">
-        <v>1.187162776348138e+134</v>
+        <v>2.1378313516241e+133</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0002341270446777344</v>
+        <v>0.0008172988891601562</v>
       </c>
     </row>
     <row r="34">
@@ -1447,31 +1447,31 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>8.697545534603832e-10</v>
+        <v>3.105944695968351e-10</v>
       </c>
       <c r="C34" t="n">
-        <v>6.377910267313109e+134</v>
+        <v>2.695425686026369e+136</v>
       </c>
       <c r="D34" t="n">
-        <v>0.02307844161987305</v>
+        <v>0.07623076438903809</v>
       </c>
       <c r="E34" t="n">
-        <v>5220.042517303313</v>
+        <v>461.1974773268069</v>
       </c>
       <c r="F34" t="n">
-        <v>6.377910271456635e+134</v>
+        <v>2.695425686081631e+136</v>
       </c>
       <c r="G34" t="n">
-        <v>0.007543563842773438</v>
+        <v>0.02615118026733398</v>
       </c>
       <c r="H34" t="n">
-        <v>5220.042515377251</v>
+        <v>461.1974773304124</v>
       </c>
       <c r="I34" t="n">
-        <v>6.377910273811176e+134</v>
+        <v>2.695425686059024e+136</v>
       </c>
       <c r="J34" t="n">
-        <v>0.01932334899902344</v>
+        <v>0.0006182193756103516</v>
       </c>
     </row>
     <row r="35">
@@ -1479,31 +1479,31 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>1.156525405383956e-11</v>
+        <v>5.01445665872147e-12</v>
       </c>
       <c r="C35" t="n">
-        <v>2.567505998246724e+144</v>
+        <v>1.453845535408806e+142</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02620077133178711</v>
+        <v>0.08283281326293945</v>
       </c>
       <c r="E35" t="n">
-        <v>9.900846754985738</v>
+        <v>7.361005079673485</v>
       </c>
       <c r="F35" t="n">
-        <v>2.567505998245769e+144</v>
+        <v>1.453845535410607e+142</v>
       </c>
       <c r="G35" t="n">
-        <v>0.007979393005371094</v>
+        <v>0.02680039405822754</v>
       </c>
       <c r="H35" t="n">
-        <v>9.900846754985199</v>
+        <v>7.361005079674096</v>
       </c>
       <c r="I35" t="n">
-        <v>2.567505998246276e+144</v>
+        <v>1.453845535410247e+142</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0002675056457519531</v>
+        <v>0.0007014274597167969</v>
       </c>
     </row>
     <row r="36">
@@ -1511,31 +1511,31 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>2.952115596975779e-09</v>
+        <v>8.796440911923961e-12</v>
       </c>
       <c r="C36" t="n">
-        <v>6.480713373933916e+145</v>
+        <v>1.765590683427461e+148</v>
       </c>
       <c r="D36" t="n">
-        <v>0.02681541442871094</v>
+        <v>0.08875942230224609</v>
       </c>
       <c r="E36" t="n">
-        <v>190.6716889818449</v>
+        <v>17.08539659180879</v>
       </c>
       <c r="F36" t="n">
-        <v>6.48071337342437e+145</v>
+        <v>1.765590683425942e+148</v>
       </c>
       <c r="G36" t="n">
-        <v>0.008424758911132812</v>
+        <v>0.02518677711486816</v>
       </c>
       <c r="H36" t="n">
-        <v>190.6716889782593</v>
+        <v>17.08539659180567</v>
       </c>
       <c r="I36" t="n">
-        <v>6.480713373551386e+145</v>
+        <v>1.76559068342624e+148</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0003042221069335938</v>
+        <v>0.0007023811340332031</v>
       </c>
     </row>
     <row r="37">
@@ -1543,31 +1543,31 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>7.72383069134307e-12</v>
+        <v>3.01243070358549e-12</v>
       </c>
       <c r="C37" t="n">
-        <v>9.867337465713849e+151</v>
+        <v>2.369848684402919e+152</v>
       </c>
       <c r="D37" t="n">
-        <v>0.02894234657287598</v>
+        <v>0.09723162651062012</v>
       </c>
       <c r="E37" t="n">
-        <v>15.61247357097661</v>
+        <v>7.075449632088208</v>
       </c>
       <c r="F37" t="n">
-        <v>9.867337465704661e+151</v>
+        <v>2.369848684402649e+152</v>
       </c>
       <c r="G37" t="n">
-        <v>0.008863449096679688</v>
+        <v>0.02067828178405762</v>
       </c>
       <c r="H37" t="n">
-        <v>15.61247357097148</v>
+        <v>7.075449632087839</v>
       </c>
       <c r="I37" t="n">
-        <v>9.867337465711356e+151</v>
+        <v>2.369848684403344e+152</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0001935958862304688</v>
+        <v>0.0006253719329833984</v>
       </c>
     </row>
     <row r="38">
@@ -1575,31 +1575,31 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>9.963262803867809e-12</v>
+        <v>5.173813826718977e-11</v>
       </c>
       <c r="C38" t="n">
-        <v>1.1468200448295e+156</v>
+        <v>1.504519029565677e+155</v>
       </c>
       <c r="D38" t="n">
-        <v>0.03051495552062988</v>
+        <v>0.1033990383148193</v>
       </c>
       <c r="E38" t="n">
-        <v>22.69474611398114</v>
+        <v>134.599332902993</v>
       </c>
       <c r="F38" t="n">
-        <v>1.146820044824589e+156</v>
+        <v>1.50451902957102e+155</v>
       </c>
       <c r="G38" t="n">
-        <v>0.009404897689819336</v>
+        <v>0.01755857467651367</v>
       </c>
       <c r="H38" t="n">
-        <v>22.69474611391563</v>
+        <v>134.5993329022063</v>
       </c>
       <c r="I38" t="n">
-        <v>1.146820044828239e+156</v>
+        <v>1.504519029579528e+155</v>
       </c>
       <c r="J38" t="n">
-        <v>0.002206802368164062</v>
+        <v>0.0006320476531982422</v>
       </c>
     </row>
     <row r="39">
@@ -1607,31 +1607,31 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>3.45774807405863e-11</v>
+        <v>5.250748867291538e-10</v>
       </c>
       <c r="C39" t="n">
-        <v>1.181908838049619e+160</v>
+        <v>6.689124258993062e+158</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03286218643188477</v>
+        <v>0.1111423969268799</v>
       </c>
       <c r="E39" t="n">
-        <v>30.59564414323118</v>
+        <v>355.6481100407262</v>
       </c>
       <c r="F39" t="n">
-        <v>1.181908838048603e+160</v>
+        <v>6.68912425865587e+158</v>
       </c>
       <c r="G39" t="n">
-        <v>0.009860038757324219</v>
+        <v>0.01349163055419922</v>
       </c>
       <c r="H39" t="n">
-        <v>30.59564414324422</v>
+        <v>355.6481100492986</v>
       </c>
       <c r="I39" t="n">
-        <v>1.181908838048345e+160</v>
+        <v>6.689124258493918e+158</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0002355575561523438</v>
+        <v>0.0006635189056396484</v>
       </c>
     </row>
     <row r="40">
@@ -1639,31 +1639,31 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>3.97604775167782e-11</v>
+        <v>4.371837543930386e-11</v>
       </c>
       <c r="C40" t="n">
-        <v>1.646815408150893e+165</v>
+        <v>1.638211851303851e+163</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0357825756072998</v>
+        <v>0.1148321628570557</v>
       </c>
       <c r="E40" t="n">
-        <v>102.3151995581126</v>
+        <v>34.72035104987337</v>
       </c>
       <c r="F40" t="n">
-        <v>1.646815408163438e+165</v>
+        <v>1.638211851310476e+163</v>
       </c>
       <c r="G40" t="n">
-        <v>0.01047849655151367</v>
+        <v>0.01378369331359863</v>
       </c>
       <c r="H40" t="n">
-        <v>102.315199557935</v>
+        <v>34.7203510500907</v>
       </c>
       <c r="I40" t="n">
-        <v>1.646815408165977e+165</v>
+        <v>1.638211851300404e+163</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0002079010009765625</v>
+        <v>0.0007598400115966797</v>
       </c>
     </row>
     <row r="41">
@@ -1671,31 +1671,31 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>4.862128308894213e-12</v>
+        <v>7.017341468512197e-11</v>
       </c>
       <c r="C41" t="n">
-        <v>7.839627956602134e+169</v>
+        <v>4.894333512348044e+168</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0363459587097168</v>
+        <v>0.1177713871002197</v>
       </c>
       <c r="E41" t="n">
-        <v>22.25536017600063</v>
+        <v>6.646382511316574</v>
       </c>
       <c r="F41" t="n">
-        <v>7.83962795664618e+169</v>
+        <v>4.894333512360015e+168</v>
       </c>
       <c r="G41" t="n">
-        <v>0.01146721839904785</v>
+        <v>0.01440739631652832</v>
       </c>
       <c r="H41" t="n">
-        <v>22.2553601759416</v>
+        <v>6.646382511316395</v>
       </c>
       <c r="I41" t="n">
-        <v>7.839627956670463e+169</v>
+        <v>4.894333512362216e+168</v>
       </c>
       <c r="J41" t="n">
-        <v>0.004471063613891602</v>
+        <v>0.0006442070007324219</v>
       </c>
     </row>
     <row r="42">
@@ -1703,31 +1703,31 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>1.215055204458513e-12</v>
+        <v>2.624521641754626e-11</v>
       </c>
       <c r="C42" t="n">
-        <v>2.739716509410741e+177</v>
+        <v>7.99335336636925e+173</v>
       </c>
       <c r="D42" t="n">
-        <v>0.04101109504699707</v>
+        <v>0.121143102645874</v>
       </c>
       <c r="E42" t="n">
-        <v>6.731027340871297</v>
+        <v>37.99330698783412</v>
       </c>
       <c r="F42" t="n">
-        <v>2.73971650941064e+177</v>
+        <v>7.993353366406235e+173</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01153063774108887</v>
+        <v>0.01522636413574219</v>
       </c>
       <c r="H42" t="n">
-        <v>6.731027340871237</v>
+        <v>37.99330698783291</v>
       </c>
       <c r="I42" t="n">
-        <v>2.739716509410884e+177</v>
+        <v>7.993353366402188e+173</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0002675056457519531</v>
+        <v>0.0006744861602783203</v>
       </c>
     </row>
     <row r="43">
@@ -1735,31 +1735,31 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>2.609511405388351e-12</v>
+        <v>9.664660220687007e-12</v>
       </c>
       <c r="C43" t="n">
-        <v>2.016951823384702e+180</v>
+        <v>7.063968543355607e+178</v>
       </c>
       <c r="D43" t="n">
-        <v>0.04121494293212891</v>
+        <v>0.1244368553161621</v>
       </c>
       <c r="E43" t="n">
-        <v>8.230238073460065</v>
+        <v>9.937182414839004</v>
       </c>
       <c r="F43" t="n">
-        <v>2.01695182338463e+180</v>
+        <v>7.06396854335425e+178</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01113677024841309</v>
+        <v>0.01594996452331543</v>
       </c>
       <c r="H43" t="n">
-        <v>8.230238073460377</v>
+        <v>9.937182414842015</v>
       </c>
       <c r="I43" t="n">
-        <v>2.016951823383919e+180</v>
+        <v>7.063968543346349e+178</v>
       </c>
       <c r="J43" t="n">
-        <v>0.003707647323608398</v>
+        <v>0.0007328987121582031</v>
       </c>
     </row>
     <row r="44">
@@ -1767,31 +1767,31 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>1.553831576328747e-12</v>
+        <v>1.498023213705614e-11</v>
       </c>
       <c r="C44" t="n">
-        <v>3.105107300543844e+183</v>
+        <v>8.615115030147718e+182</v>
       </c>
       <c r="D44" t="n">
-        <v>0.04690766334533691</v>
+        <v>0.1278715133666992</v>
       </c>
       <c r="E44" t="n">
-        <v>8.82870939495468</v>
+        <v>31.61431510411832</v>
       </c>
       <c r="F44" t="n">
-        <v>3.105107300544484e+183</v>
+        <v>8.615115030155883e+182</v>
       </c>
       <c r="G44" t="n">
-        <v>0.01293778419494629</v>
+        <v>0.0165708065032959</v>
       </c>
       <c r="H44" t="n">
-        <v>8.828709394954851</v>
+        <v>31.61431510409636</v>
       </c>
       <c r="I44" t="n">
-        <v>3.105107300543561e+183</v>
+        <v>8.615115030165242e+182</v>
       </c>
       <c r="J44" t="n">
-        <v>0.002388477325439453</v>
+        <v>0.0007185935974121094</v>
       </c>
     </row>
     <row r="45">
@@ -1799,31 +1799,31 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>1.765618278835887e-11</v>
+        <v>4.097508909070425e-11</v>
       </c>
       <c r="C45" t="n">
-        <v>3.502773810759635e+188</v>
+        <v>7.246951785737503e+188</v>
       </c>
       <c r="D45" t="n">
-        <v>0.04789161682128906</v>
+        <v>0.1313486099243164</v>
       </c>
       <c r="E45" t="n">
-        <v>13.79620328815041</v>
+        <v>15.89129539973447</v>
       </c>
       <c r="F45" t="n">
-        <v>3.502773810752344e+188</v>
+        <v>7.246951785762644e+188</v>
       </c>
       <c r="G45" t="n">
-        <v>0.01355624198913574</v>
+        <v>0.01738739013671875</v>
       </c>
       <c r="H45" t="n">
-        <v>13.79620328813679</v>
+        <v>15.89129539977557</v>
       </c>
       <c r="I45" t="n">
-        <v>3.502773810757115e+188</v>
+        <v>7.246951785740815e+188</v>
       </c>
       <c r="J45" t="n">
-        <v>0.01420021057128906</v>
+        <v>0.0007297992706298828</v>
       </c>
     </row>
     <row r="46">
@@ -1831,31 +1831,31 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>1.060094484890893e-11</v>
+        <v>2.860356819738567e-11</v>
       </c>
       <c r="C46" t="n">
-        <v>2.098594214371075e+193</v>
+        <v>1.919626147625865e+191</v>
       </c>
       <c r="D46" t="n">
-        <v>0.05300378799438477</v>
+        <v>0.1358356475830078</v>
       </c>
       <c r="E46" t="n">
-        <v>8.246810972491643</v>
+        <v>72.3826083512611</v>
       </c>
       <c r="F46" t="n">
-        <v>2.098594214373013e+193</v>
+        <v>1.919626147627901e+191</v>
       </c>
       <c r="G46" t="n">
-        <v>0.01386189460754395</v>
+        <v>0.0182192325592041</v>
       </c>
       <c r="H46" t="n">
-        <v>8.246810972491607</v>
+        <v>72.38260835150606</v>
       </c>
       <c r="I46" t="n">
-        <v>2.098594214373903e+193</v>
+        <v>1.919626147621392e+191</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0006158351898193359</v>
+        <v>0.0007231235504150391</v>
       </c>
     </row>
     <row r="47">
@@ -1863,31 +1863,31 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>2.833776104147416e-11</v>
+        <v>1.032460060826265e-10</v>
       </c>
       <c r="C47" t="n">
-        <v>1.856473146826689e+197</v>
+        <v>2.210676738877179e+196</v>
       </c>
       <c r="D47" t="n">
-        <v>0.05462002754211426</v>
+        <v>0.139704704284668</v>
       </c>
       <c r="E47" t="n">
-        <v>75.39562718105854</v>
+        <v>54.04048580165358</v>
       </c>
       <c r="F47" t="n">
-        <v>1.856473146830697e+197</v>
+        <v>2.210676738922499e+196</v>
       </c>
       <c r="G47" t="n">
-        <v>0.01446223258972168</v>
+        <v>0.01881527900695801</v>
       </c>
       <c r="H47" t="n">
-        <v>75.39562718063618</v>
+        <v>54.04048580149276</v>
       </c>
       <c r="I47" t="n">
-        <v>1.856473146845018e+197</v>
+        <v>2.210676738928625e+196</v>
       </c>
       <c r="J47" t="n">
-        <v>0.002922534942626953</v>
+        <v>0.0008306503295898438</v>
       </c>
     </row>
     <row r="48">
@@ -1895,31 +1895,31 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>1.137198848054318e-11</v>
+        <v>2.276270913156851e-11</v>
       </c>
       <c r="C48" t="n">
-        <v>1.922745016102448e+199</v>
+        <v>5.91593098543525e+201</v>
       </c>
       <c r="D48" t="n">
-        <v>0.05800080299377441</v>
+        <v>0.1436591148376465</v>
       </c>
       <c r="E48" t="n">
-        <v>292.4459021324018</v>
+        <v>14.49877195046517</v>
       </c>
       <c r="F48" t="n">
-        <v>1.922745016103248e+199</v>
+        <v>5.915930985429977e+201</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0148160457611084</v>
+        <v>0.01938891410827637</v>
       </c>
       <c r="H48" t="n">
-        <v>292.445902129403</v>
+        <v>14.49877195046358</v>
       </c>
       <c r="I48" t="n">
-        <v>1.922745016123422e+199</v>
+        <v>5.915930985431734e+201</v>
       </c>
       <c r="J48" t="n">
-        <v>0.0007145404815673828</v>
+        <v>0.004806041717529297</v>
       </c>
     </row>
     <row r="49">
@@ -1927,31 +1927,31 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>1.96733272391441e-11</v>
+        <v>1.969689025972903e-11</v>
       </c>
       <c r="C49" t="n">
-        <v>1.039090346757568e+207</v>
+        <v>5.297493843525267e+206</v>
       </c>
       <c r="D49" t="n">
-        <v>0.06125378608703613</v>
+        <v>0.1485545635223389</v>
       </c>
       <c r="E49" t="n">
-        <v>20.43626845483987</v>
+        <v>7.508636050495705</v>
       </c>
       <c r="F49" t="n">
-        <v>1.039090346756297e+207</v>
+        <v>5.297493843524861e+206</v>
       </c>
       <c r="G49" t="n">
-        <v>0.01511693000793457</v>
+        <v>0.02048611640930176</v>
       </c>
       <c r="H49" t="n">
-        <v>20.43626845485112</v>
+        <v>7.508636050495477</v>
       </c>
       <c r="I49" t="n">
-        <v>1.039090346755682e+207</v>
+        <v>5.297493843522115e+206</v>
       </c>
       <c r="J49" t="n">
-        <v>0.003651142120361328</v>
+        <v>0.0008249282836914062</v>
       </c>
     </row>
     <row r="50">
@@ -1959,31 +1959,31 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>4.862936514571985e-12</v>
+        <v>4.3031895282808e-12</v>
       </c>
       <c r="C50" t="n">
-        <v>7.501344654747801e+212</v>
+        <v>2.002521468460234e+212</v>
       </c>
       <c r="D50" t="n">
-        <v>0.06592416763305664</v>
+        <v>0.1532022953033447</v>
       </c>
       <c r="E50" t="n">
-        <v>9.031916940090925</v>
+        <v>11.14394143131779</v>
       </c>
       <c r="F50" t="n">
-        <v>7.501344654748516e+212</v>
+        <v>2.00252146846064e+212</v>
       </c>
       <c r="G50" t="n">
-        <v>0.01635169982910156</v>
+        <v>0.02152252197265625</v>
       </c>
       <c r="H50" t="n">
-        <v>9.031916940090747</v>
+        <v>11.14394143131716</v>
       </c>
       <c r="I50" t="n">
-        <v>7.501344654748873e+212</v>
+        <v>2.002521468460571e+212</v>
       </c>
       <c r="J50" t="n">
-        <v>0.00035858154296875</v>
+        <v>0.0008733272552490234</v>
       </c>
     </row>
     <row r="51">
@@ -1991,31 +1991,31 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>1.8354862742594e-12</v>
+        <v>2.740133084742954e-12</v>
       </c>
       <c r="C51" t="n">
-        <v>3.56502276811121e+217</v>
+        <v>1.490221051376379e+215</v>
       </c>
       <c r="D51" t="n">
-        <v>0.07045769691467285</v>
+        <v>0.157447338104248</v>
       </c>
       <c r="E51" t="n">
-        <v>7.38188461168671</v>
+        <v>379.1144436496068</v>
       </c>
       <c r="F51" t="n">
-        <v>3.565022768111285e+217</v>
+        <v>1.490221051332847e+215</v>
       </c>
       <c r="G51" t="n">
-        <v>0.01696372032165527</v>
+        <v>0.02207016944885254</v>
       </c>
       <c r="H51" t="n">
-        <v>7.381884611686795</v>
+        <v>379.1144436637933</v>
       </c>
       <c r="I51" t="n">
-        <v>3.565022768111797e+217</v>
+        <v>1.490221051277028e+215</v>
       </c>
       <c r="J51" t="n">
-        <v>0.0003619194030761719</v>
+        <v>0.001108169555664062</v>
       </c>
     </row>
     <row r="52">
@@ -2023,31 +2023,31 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>4.747069680867027e-11</v>
+        <v>2.074365778782539e-10</v>
       </c>
       <c r="C52" t="n">
-        <v>7.898486277249778e+218</v>
+        <v>1.263719008362549e+219</v>
       </c>
       <c r="D52" t="n">
-        <v>0.07393193244934082</v>
+        <v>0.1629352569580078</v>
       </c>
       <c r="E52" t="n">
-        <v>26.57285857193972</v>
+        <v>191.398308080327</v>
       </c>
       <c r="F52" t="n">
-        <v>7.898486277299917e+218</v>
+        <v>1.263719008423649e+219</v>
       </c>
       <c r="G52" t="n">
-        <v>0.01766681671142578</v>
+        <v>0.02413678169250488</v>
       </c>
       <c r="H52" t="n">
-        <v>26.57285857204568</v>
+        <v>191.3983080794215</v>
       </c>
       <c r="I52" t="n">
-        <v>7.898486277263691e+218</v>
+        <v>1.263719008427545e+219</v>
       </c>
       <c r="J52" t="n">
-        <v>0.0004034042358398438</v>
+        <v>0.03513193130493164</v>
       </c>
     </row>
     <row r="53">
@@ -2055,31 +2055,31 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>8.366385716387523e-12</v>
+        <v>1.263450613992982e-10</v>
       </c>
       <c r="C53" t="n">
-        <v>2.153180639734884e+225</v>
+        <v>3.983961935369087e+224</v>
       </c>
       <c r="D53" t="n">
-        <v>0.07829594612121582</v>
+        <v>0.1683664321899414</v>
       </c>
       <c r="E53" t="n">
-        <v>8.380340325102752</v>
+        <v>43.88282867004111</v>
       </c>
       <c r="F53" t="n">
-        <v>2.153180639737639e+225</v>
+        <v>3.983961935396907e+224</v>
       </c>
       <c r="G53" t="n">
-        <v>0.01834440231323242</v>
+        <v>0.02382588386535645</v>
       </c>
       <c r="H53" t="n">
-        <v>8.380340325103706</v>
+        <v>43.88282867006084</v>
       </c>
       <c r="I53" t="n">
-        <v>2.153180639736777e+225</v>
+        <v>3.983961935395234e+224</v>
       </c>
       <c r="J53" t="n">
-        <v>0.0003948211669921875</v>
+        <v>0.0009894371032714844</v>
       </c>
     </row>
     <row r="54">
@@ -2087,31 +2087,31 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>6.52722784046799e-11</v>
+        <v>5.025673243582561e-11</v>
       </c>
       <c r="C54" t="n">
-        <v>1.049539670704603e+228</v>
+        <v>1.112791548252025e+229</v>
       </c>
       <c r="D54" t="n">
-        <v>0.08091521263122559</v>
+        <v>0.1726870536804199</v>
       </c>
       <c r="E54" t="n">
-        <v>121.4191265306944</v>
+        <v>49.3953712218971</v>
       </c>
       <c r="F54" t="n">
-        <v>1.049539670709633e+228</v>
+        <v>1.112791548262774e+229</v>
       </c>
       <c r="G54" t="n">
-        <v>0.01901984214782715</v>
+        <v>0.02480411529541016</v>
       </c>
       <c r="H54" t="n">
-        <v>121.4191265308976</v>
+        <v>49.39537122195841</v>
       </c>
       <c r="I54" t="n">
-        <v>1.049539670707734e+228</v>
+        <v>1.112791548263229e+229</v>
       </c>
       <c r="J54" t="n">
-        <v>0.0003266334533691406</v>
+        <v>0.001005172729492188</v>
       </c>
     </row>
     <row r="55">
@@ -2119,31 +2119,31 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>1.035641040199761e-10</v>
+        <v>9.094946175439681e-12</v>
       </c>
       <c r="C55" t="n">
-        <v>7.593708587441998e+231</v>
+        <v>1.13522748559808e+235</v>
       </c>
       <c r="D55" t="n">
-        <v>0.08685779571533203</v>
+        <v>0.1786191463470459</v>
       </c>
       <c r="E55" t="n">
-        <v>235.6434974582012</v>
+        <v>28.96687322679036</v>
       </c>
       <c r="F55" t="n">
-        <v>7.593708588082897e+231</v>
+        <v>1.135227485599866e+235</v>
       </c>
       <c r="G55" t="n">
-        <v>0.02036213874816895</v>
+        <v>0.02598381042480469</v>
       </c>
       <c r="H55" t="n">
-        <v>235.6434974662604</v>
+        <v>28.96687322678742</v>
       </c>
       <c r="I55" t="n">
-        <v>7.593708587830993e+231</v>
+        <v>1.135227485600003e+235</v>
       </c>
       <c r="J55" t="n">
-        <v>0.0005300045013427734</v>
+        <v>0.005704641342163086</v>
       </c>
     </row>
     <row r="56">
@@ -2151,31 +2151,31 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>1.483931103156787e-11</v>
+        <v>6.494579750141402e-10</v>
       </c>
       <c r="C56" t="n">
-        <v>5.500011880671953e+240</v>
+        <v>2.776661485253683e+238</v>
       </c>
       <c r="D56" t="n">
-        <v>0.09018826484680176</v>
+        <v>0.1836419105529785</v>
       </c>
       <c r="E56" t="n">
-        <v>10.02868994592199</v>
+        <v>372.1207378272754</v>
       </c>
       <c r="F56" t="n">
-        <v>5.500011880663746e+240</v>
+        <v>2.776661484694031e+238</v>
       </c>
       <c r="G56" t="n">
-        <v>0.02034425735473633</v>
+        <v>0.0264589786529541</v>
       </c>
       <c r="H56" t="n">
-        <v>10.02868994592143</v>
+        <v>372.120737842547</v>
       </c>
       <c r="I56" t="n">
-        <v>5.500011880670057e+240</v>
+        <v>2.776661484578275e+238</v>
       </c>
       <c r="J56" t="n">
-        <v>0.0003185272216796875</v>
+        <v>0.001005172729492188</v>
       </c>
     </row>
     <row r="57">
@@ -2183,31 +2183,31 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>1.326568344176217e-10</v>
+        <v>5.058430592595643e-10</v>
       </c>
       <c r="C57" t="n">
-        <v>1.188202830668417e+244</v>
+        <v>3.993936882448448e+240</v>
       </c>
       <c r="D57" t="n">
-        <v>0.09617519378662109</v>
+        <v>0.189544677734375</v>
       </c>
       <c r="E57" t="n">
-        <v>67.53272854609624</v>
+        <v>1282.897102656837</v>
       </c>
       <c r="F57" t="n">
-        <v>1.188202830703204e+244</v>
+        <v>3.993936882411703e+240</v>
       </c>
       <c r="G57" t="n">
-        <v>0.01782131195068359</v>
+        <v>0.02742981910705566</v>
       </c>
       <c r="H57" t="n">
-        <v>67.53272854779077</v>
+        <v>1282.897102650699</v>
       </c>
       <c r="I57" t="n">
-        <v>1.188202830673829e+244</v>
+        <v>3.9939368824393e+240</v>
       </c>
       <c r="J57" t="n">
-        <v>0.0003950595855712891</v>
+        <v>0.0009794235229492188</v>
       </c>
     </row>
     <row r="58">
@@ -2215,31 +2215,31 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>1.628981282090554e-10</v>
+        <v>2.866168809487105e-11</v>
       </c>
       <c r="C58" t="n">
-        <v>1.457912223167472e+248</v>
+        <v>1.272193719888953e+248</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1011786460876465</v>
+        <v>0.1966814994812012</v>
       </c>
       <c r="E58" t="n">
-        <v>14.72923135778109</v>
+        <v>12.78246080230259</v>
       </c>
       <c r="F58" t="n">
-        <v>1.45791222315702e+248</v>
+        <v>1.272193719887364e+248</v>
       </c>
       <c r="G58" t="n">
-        <v>0.01481080055236816</v>
+        <v>0.02910518646240234</v>
       </c>
       <c r="H58" t="n">
-        <v>14.72923135781446</v>
+        <v>12.78246080230515</v>
       </c>
       <c r="I58" t="n">
-        <v>1.457912223150358e+248</v>
+        <v>1.272193719886774e+248</v>
       </c>
       <c r="J58" t="n">
-        <v>0.00083160400390625</v>
+        <v>0.001204729080200195</v>
       </c>
     </row>
     <row r="59">
@@ -2247,31 +2247,31 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>6.251502061239744e-11</v>
+        <v>2.01718610136764e-09</v>
       </c>
       <c r="C59" t="n">
-        <v>3.166144665723717e+254</v>
+        <v>1.517705950065889e+251</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1043810844421387</v>
+        <v>0.2020416259765625</v>
       </c>
       <c r="E59" t="n">
-        <v>9.200823775127873</v>
+        <v>1781.343882134711</v>
       </c>
       <c r="F59" t="n">
-        <v>3.166144665728302e+254</v>
+        <v>1.517705949771453e+251</v>
       </c>
       <c r="G59" t="n">
-        <v>0.01416158676147461</v>
+        <v>0.02952218055725098</v>
       </c>
       <c r="H59" t="n">
-        <v>9.200823775128814</v>
+        <v>1781.343881917635</v>
       </c>
       <c r="I59" t="n">
-        <v>3.166144665726573e+254</v>
+        <v>1.517705949957156e+251</v>
       </c>
       <c r="J59" t="n">
-        <v>0.0004243850708007812</v>
+        <v>0.00110316276550293</v>
       </c>
     </row>
     <row r="60">
@@ -2279,31 +2279,31 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>1.817299364537265e-10</v>
+        <v>9.806506499406179e-11</v>
       </c>
       <c r="C60" t="n">
-        <v>5.534057240407507e+257</v>
+        <v>1.312905592936509e+256</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0988304615020752</v>
+        <v>0.2077033519744873</v>
       </c>
       <c r="E60" t="n">
-        <v>9.728171298717761</v>
+        <v>65.57415613827138</v>
       </c>
       <c r="F60" t="n">
-        <v>5.534057240272995e+257</v>
+        <v>1.312905592919926e+256</v>
       </c>
       <c r="G60" t="n">
-        <v>0.01743006706237793</v>
+        <v>0.03049516677856445</v>
       </c>
       <c r="H60" t="n">
-        <v>9.72817129868155</v>
+        <v>65.57415613765377</v>
       </c>
       <c r="I60" t="n">
-        <v>5.534057240311608e+257</v>
+        <v>1.312905592934021e+256</v>
       </c>
       <c r="J60" t="n">
-        <v>0.002891778945922852</v>
+        <v>0.001090288162231445</v>
       </c>
     </row>
     <row r="61">
@@ -2311,31 +2311,31 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>4.057940060769304e-10</v>
+        <v>9.141994835530057e-11</v>
       </c>
       <c r="C61" t="n">
-        <v>6.189966043372978e+259</v>
+        <v>1.642691316028561e+261</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1133708953857422</v>
+        <v>0.2163259983062744</v>
       </c>
       <c r="E61" t="n">
-        <v>57.6938252617444</v>
+        <v>45.54755349265147</v>
       </c>
       <c r="F61" t="n">
-        <v>6.189966043407486e+259</v>
+        <v>1.642691316019569e+261</v>
       </c>
       <c r="G61" t="n">
-        <v>0.008632659912109375</v>
+        <v>0.03195762634277344</v>
       </c>
       <c r="H61" t="n">
-        <v>57.69382526167058</v>
+        <v>45.54755349233863</v>
       </c>
       <c r="I61" t="n">
-        <v>6.189966043445093e+259</v>
+        <v>1.642691316031867e+261</v>
       </c>
       <c r="J61" t="n">
-        <v>0.0004382133483886719</v>
+        <v>0.001226663589477539</v>
       </c>
     </row>
     <row r="62">
@@ -2343,31 +2343,31 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>5.279981632262385e-10</v>
+        <v>1.098619746559465e-10</v>
       </c>
       <c r="C62" t="n">
-        <v>1.700120873034899e+263</v>
+        <v>1.147039613231287e+268</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1121630668640137</v>
+        <v>0.2238686084747314</v>
       </c>
       <c r="E62" t="n">
-        <v>433.960312674315</v>
+        <v>10.88715314089646</v>
       </c>
       <c r="F62" t="n">
-        <v>1.700120873019066e+263</v>
+        <v>1.147039613238989e+268</v>
       </c>
       <c r="G62" t="n">
-        <v>0.0122833251953125</v>
+        <v>0.03306818008422852</v>
       </c>
       <c r="H62" t="n">
-        <v>433.9603126542453</v>
+        <v>10.8871531408999</v>
       </c>
       <c r="I62" t="n">
-        <v>1.70012087309185e+263</v>
+        <v>1.147039613234147e+268</v>
       </c>
       <c r="J62" t="n">
-        <v>0.0004208087921142578</v>
+        <v>0.001213312149047852</v>
       </c>
     </row>
     <row r="63">
@@ -2375,31 +2375,31 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>3.157155904591938e-11</v>
+        <v>3.788285933663957e-11</v>
       </c>
       <c r="C63" t="n">
-        <v>3.113011685418058e+271</v>
+        <v>1.067815295186025e+273</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1165952682495117</v>
+        <v>0.2287552356719971</v>
       </c>
       <c r="E63" t="n">
-        <v>50.87779043753925</v>
+        <v>8.63628072949982</v>
       </c>
       <c r="F63" t="n">
-        <v>3.113011685388426e+271</v>
+        <v>1.067815295187256e+273</v>
       </c>
       <c r="G63" t="n">
-        <v>0.009117364883422852</v>
+        <v>0.03386235237121582</v>
       </c>
       <c r="H63" t="n">
-        <v>50.87779043738066</v>
+        <v>8.636280729500566</v>
       </c>
       <c r="I63" t="n">
-        <v>3.113011685404813e+271</v>
+        <v>1.067815295185313e+273</v>
       </c>
       <c r="J63" t="n">
-        <v>0.0003809928894042969</v>
+        <v>0.001281261444091797</v>
       </c>
     </row>
     <row r="64">
@@ -2407,31 +2407,31 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>7.323796396349604e-11</v>
+        <v>6.745700732414398e-09</v>
       </c>
       <c r="C64" t="n">
-        <v>2.758256390477529e+276</v>
+        <v>7.089104833338667e+271</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1228659152984619</v>
+        <v>0.2418851852416992</v>
       </c>
       <c r="E64" t="n">
-        <v>28.08868914440245</v>
+        <v>278751.2654916889</v>
       </c>
       <c r="F64" t="n">
-        <v>2.758256390466685e+276</v>
+        <v>7.089104894339165e+271</v>
       </c>
       <c r="G64" t="n">
-        <v>0.01842093467712402</v>
+        <v>0.03534293174743652</v>
       </c>
       <c r="H64" t="n">
-        <v>28.0886891444565</v>
+        <v>278751.2579561005</v>
       </c>
       <c r="I64" t="n">
-        <v>2.758256390459917e+276</v>
+        <v>7.089105085981094e+271</v>
       </c>
       <c r="J64" t="n">
-        <v>0.003301382064819336</v>
+        <v>0.001274585723876953</v>
       </c>
     </row>
     <row r="65">
@@ -2439,31 +2439,31 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>1.638443269434369e-11</v>
+        <v>5.712941670103524e-10</v>
       </c>
       <c r="C65" t="n">
-        <v>1.960730711846066e+280</v>
+        <v>3.496965993789412e+281</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1202895641326904</v>
+        <v>0.2433123588562012</v>
       </c>
       <c r="E65" t="n">
-        <v>15.73776832270793</v>
+        <v>78.38729231667178</v>
       </c>
       <c r="F65" t="n">
-        <v>1.960730711834563e+280</v>
+        <v>3.496965993905295e+281</v>
       </c>
       <c r="G65" t="n">
-        <v>0.009759426116943359</v>
+        <v>0.03588414192199707</v>
       </c>
       <c r="H65" t="n">
-        <v>15.73776832269585</v>
+        <v>78.38729231795546</v>
       </c>
       <c r="I65" t="n">
-        <v>1.960730711836487e+280</v>
+        <v>3.496965993844673e+281</v>
       </c>
       <c r="J65" t="n">
-        <v>0.0004172325134277344</v>
+        <v>0.001153707504272461</v>
       </c>
     </row>
     <row r="66">
@@ -2471,31 +2471,31 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>2.723790344005749e-10</v>
+        <v>5.471227847298334e-10</v>
       </c>
       <c r="C66" t="n">
-        <v>2.652049269259207e+286</v>
+        <v>2.381333993964235e+285</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1237945556640625</v>
+        <v>0.251274585723877</v>
       </c>
       <c r="E66" t="n">
-        <v>81.95372824012281</v>
+        <v>4345.433353642348</v>
       </c>
       <c r="F66" t="n">
-        <v>2.652049269235407e+286</v>
+        <v>2.381333994035456e+285</v>
       </c>
       <c r="G66" t="n">
-        <v>0.01140427589416504</v>
+        <v>0.03703427314758301</v>
       </c>
       <c r="H66" t="n">
-        <v>81.95372823990033</v>
+        <v>4345.433353759417</v>
       </c>
       <c r="I66" t="n">
-        <v>2.652049269244549e+286</v>
+        <v>2.381333993972221e+285</v>
       </c>
       <c r="J66" t="n">
-        <v>0.0004334449768066406</v>
+        <v>0.001127243041992188</v>
       </c>
     </row>
     <row r="67">
@@ -2503,31 +2503,31 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>8.258971726921731e-11</v>
+        <v>1.431319695342086e-11</v>
       </c>
       <c r="C67" t="n">
-        <v>3.057827489135899e+290</v>
+        <v>4.476774800426501e+291</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1246926784515381</v>
+        <v>0.2575132846832275</v>
       </c>
       <c r="E67" t="n">
-        <v>24.58602251110274</v>
+        <v>16.83528183188963</v>
       </c>
       <c r="F67" t="n">
-        <v>3.057827489139069e+290</v>
+        <v>4.476774800427267e+291</v>
       </c>
       <c r="G67" t="n">
-        <v>0.01016759872436523</v>
+        <v>0.03891205787658691</v>
       </c>
       <c r="H67" t="n">
-        <v>24.58602251107363</v>
+        <v>16.83528183189496</v>
       </c>
       <c r="I67" t="n">
-        <v>3.05782748914355e+290</v>
+        <v>4.476774800429364e+291</v>
       </c>
       <c r="J67" t="n">
-        <v>0.0003693103790283203</v>
+        <v>0.001274824142456055</v>
       </c>
     </row>
     <row r="68">
@@ -2535,31 +2535,31 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>1.173484275211031e-10</v>
+        <v>8.158678689840397e-11</v>
       </c>
       <c r="C68" t="n">
-        <v>1.71252924895886e+294</v>
+        <v>1.150051037170681e+297</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1280815601348877</v>
+        <v>0.268763542175293</v>
       </c>
       <c r="E68" t="n">
-        <v>179.3749359266677</v>
+        <v>23.11309442833062</v>
       </c>
       <c r="F68" t="n">
-        <v>1.712529248950993e+294</v>
+        <v>1.15005103717525e+297</v>
       </c>
       <c r="G68" t="n">
-        <v>0.01177024841308594</v>
+        <v>0.0390174388885498</v>
       </c>
       <c r="H68" t="n">
-        <v>179.3749359270734</v>
+        <v>23.11309442826623</v>
       </c>
       <c r="I68" t="n">
-        <v>1.712529248949956e+294</v>
+        <v>1.150051037177738e+297</v>
       </c>
       <c r="J68" t="n">
-        <v>0.0004107952117919922</v>
+        <v>0.001272916793823242</v>
       </c>
     </row>
     <row r="69">
@@ -2567,31 +2567,31 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>4.97287819328355e-11</v>
+        <v>3.249743726227387e-09</v>
       </c>
       <c r="C69" t="n">
-        <v>5.708479779142257e+299</v>
+        <v>3.01060747635572e+298</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1289312839508057</v>
+        <v>0.2754220962524414</v>
       </c>
       <c r="E69" t="n">
-        <v>29.50369576382774</v>
+        <v>418.6815580920563</v>
       </c>
       <c r="F69" t="n">
-        <v>5.708479779157505e+299</v>
+        <v>3.010607476445266e+298</v>
       </c>
       <c r="G69" t="n">
-        <v>0.0109550952911377</v>
+        <v>0.04047608375549316</v>
       </c>
       <c r="H69" t="n">
-        <v>29.50369576387726</v>
+        <v>418.681558089424</v>
       </c>
       <c r="I69" t="n">
-        <v>5.708479779131563e+299</v>
+        <v>3.01060747646377e+298</v>
       </c>
       <c r="J69" t="n">
-        <v>0.0003755092620849609</v>
+        <v>0.001282930374145508</v>
       </c>
     </row>
     <row r="70">
@@ -2599,31 +2599,31 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>6.746869671983728e-11</v>
+        <v>6.792375337324895e-10</v>
       </c>
       <c r="C70" t="n">
-        <v>1.060013809202805e+304</v>
+        <v>2.846828665188453e+305</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1338894367218018</v>
+        <v>0.283944845199585</v>
       </c>
       <c r="E70" t="n">
-        <v>63.35975391480676</v>
+        <v>183.091999350507</v>
       </c>
       <c r="F70" t="n">
-        <v>1.060013809210319e+304</v>
+        <v>2.846828664924985e+305</v>
       </c>
       <c r="G70" t="n">
-        <v>0.01202702522277832</v>
+        <v>0.04175114631652832</v>
       </c>
       <c r="H70" t="n">
-        <v>63.35975391496337</v>
+        <v>183.0919993484626</v>
       </c>
       <c r="I70" t="n">
-        <v>1.060013809206765e+304</v>
+        <v>2.846828664952705e+305</v>
       </c>
       <c r="J70" t="n">
-        <v>0.0004761219024658203</v>
+        <v>0.00117802619934082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>